<commit_message>
Updated algo to ensure keeping old values of count
</commit_message>
<xml_diff>
--- a/a2_q3.xlsx
+++ b/a2_q3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CurtisLui/Documents/Documents/SFU /4th Year/SUMMER 2020/CMPT 310/aima-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B55E3F9-06DD-5647-8A97-D8763D4F5E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F62E17-2C05-9847-A537-C2DCBE5ECB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="37900" windowHeight="21140" xr2:uid="{1288A5A1-1CE0-7045-B338-BAE7755F7C25}"/>
   </bookViews>
@@ -81,12 +81,6 @@
     <t>rand_graph(0.6, 31)</t>
   </si>
   <si>
-    <t>Graph Discussion</t>
-  </si>
-  <si>
-    <t>From the graphs above, we can see that the number of CSP variables assigned and unassigned are strongly correlated. When the number assigned variables increases, the number of unassigned variables increase. This verfies that our backtracking search is working correctly because when backtracking it will unassign variables, thus increasing the number of times we need to assign variables in order to reach the final solution.</t>
-  </si>
-  <si>
     <t>Question 3: Exact - Ran with Backtracking Search</t>
   </si>
   <si>
@@ -94,6 +88,13 @@
 - Minimum-remaining-values heuristic
 - least-constraining-values heuristic
 - forward checking</t>
+  </si>
+  <si>
+    <t>Result Discussion</t>
+  </si>
+  <si>
+    <t>From the graphs above, we can see that the number of CSP variables assigned and unassigned are strongly correlated. When the number of assigned variables increases, the number of unassigned variables increases. This verifies that our backtracking search is working correctly because when backtracking it will unassign variables, thus increasing the number of times we need to assign variables in order to reach the final solution.
+We can also see that the number of variables assigned and unassigned is proportional to the running time of the algorithm. This means that the longer backtracking search is running, the more CSP variables are being assigned and unassigned.</t>
   </si>
 </sst>
 </file>
@@ -234,28 +235,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="42"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="42"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,19 +409,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -467,19 +466,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -942,19 +941,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>19893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>274</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71</c:v>
+                  <c:v>589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,19 +998,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>16925</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41</c:v>
+                  <c:v>467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1474,19 +1473,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>326</c:v>
+                  <c:v>2551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>16933</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65</c:v>
+                  <c:v>5389</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92</c:v>
+                  <c:v>14950</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122</c:v>
+                  <c:v>4407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,19 +1530,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>251</c:v>
+                  <c:v>2026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>14678</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>4434</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>12028</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>3654</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,19 +2000,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>80567</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>332</c:v>
+                  <c:v>39302</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86</c:v>
+                  <c:v>54602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>12545</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57</c:v>
+                  <c:v>69103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2058,19 +2057,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>67853</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>33346</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>43640</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>10644</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>57126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2486,7 +2485,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18355781105616473"/>
+          <c:y val="0.27271889400921662"/>
+          <c:w val="0.7803927029661607"/>
+          <c:h val="0.44028375485322402"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2523,19 +2532,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>82</c:v>
+                  <c:v>456827</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93</c:v>
+                  <c:v>5594237</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5326</c:v>
+                  <c:v>1380314</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>29281831</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>2980276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2580,19 +2589,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>376609</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>4666384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4277</c:v>
+                  <c:v>1099275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>24789700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2406045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6173,67 +6182,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFCA1D8-37C5-FA4D-BDD1-DACA3CAE6D4E}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I80" sqref="I80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="A2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -6275,7 +6284,7 @@
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="10">
         <v>3</v>
       </c>
       <c r="D5" s="1">
@@ -6311,39 +6320,39 @@
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>2.6590824127197201E-3</v>
-      </c>
-      <c r="C6" s="9">
-        <v>5.2921772003173802E-3</v>
-      </c>
-      <c r="D6" s="9">
-        <v>8.0671310424804601E-3</v>
-      </c>
-      <c r="E6" s="9">
-        <v>2.48193740844726E-3</v>
-      </c>
-      <c r="F6" s="9">
-        <v>4.1010379791259696E-3</v>
+      <c r="B6" s="10">
+        <v>3.15213203430175E-3</v>
+      </c>
+      <c r="C6" s="10">
+        <v>3.3636093139648398E-3</v>
+      </c>
+      <c r="D6" s="10">
+        <v>3.0789375305175699E-3</v>
+      </c>
+      <c r="E6" s="10">
+        <v>3.9579868316650304E-3</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2.8841495513915998E-3</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ref="I6:I9" si="0">MIN(B6:F6)</f>
-        <v>2.48193740844726E-3</v>
+        <v>2.8841495513915998E-3</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" ref="J6:J9" si="1">MAX(B6:F6)</f>
-        <v>8.0671310424804601E-3</v>
+        <v>3.9579868316650304E-3</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" ref="K6:K9" si="2">AVERAGE(B6:F6)</f>
-        <v>4.5202732086181575E-3</v>
+        <v>3.2873630523681577E-3</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ref="L6:L9" si="3">MEDIAN(B6:F6)</f>
-        <v>4.1010379791259696E-3</v>
+        <v>3.15213203430175E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -6351,38 +6360,38 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>31.8</v>
+        <v>43.6</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -6390,38 +6399,38 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>12.6</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -6429,19 +6438,19 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1">
         <v>44</v>
       </c>
       <c r="E9" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
@@ -6452,11 +6461,11 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>44.8</v>
+        <v>43.2</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
@@ -6465,20 +6474,20 @@
     </row>
     <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
     </row>
     <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -6556,39 +6565,39 @@
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1">
-        <v>1.40347480773925E-2</v>
-      </c>
-      <c r="C14" s="9">
-        <v>1.11260414123535E-2</v>
-      </c>
-      <c r="D14" s="9">
-        <v>4.2845010757446199E-2</v>
-      </c>
-      <c r="E14" s="9">
-        <v>1.39451026916503E-2</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1.1603832244873E-2</v>
+      <c r="B14" s="10">
+        <v>9.7098350524902292E-3</v>
+      </c>
+      <c r="C14" s="10">
+        <v>4.6918392181396398E-3</v>
+      </c>
+      <c r="D14" s="10">
+        <v>7.3800086975097604E-3</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1.7014980316162099E-2</v>
+      </c>
+      <c r="F14" s="10">
+        <v>5.38396835327148E-3</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" ref="I14:I17" si="4">MIN(B14:F14)</f>
-        <v>1.11260414123535E-2</v>
+        <v>4.6918392181396398E-3</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" ref="J14:J17" si="5">MAX(B14:F14)</f>
-        <v>4.2845010757446199E-2</v>
+        <v>1.7014980316162099E-2</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" ref="K14:K17" si="6">AVERAGE(B14:F14)</f>
-        <v>1.87109470367431E-2</v>
+        <v>8.8361263275146418E-3</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" ref="L14:L17" si="7">MEDIAN(B14:F14)</f>
-        <v>1.39451026916503E-2</v>
+        <v>7.3800086975097604E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -6596,38 +6605,38 @@
         <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>65</v>
+        <v>148</v>
       </c>
       <c r="C15" s="1">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="E15" s="1">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="F15" s="1">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="4"/>
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="5"/>
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="K15" s="1">
         <f t="shared" si="6"/>
-        <v>38.4</v>
+        <v>120.4</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="7"/>
-        <v>31</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -6635,38 +6644,38 @@
         <v>3</v>
       </c>
       <c r="B16" s="1">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" si="6"/>
-        <v>6.6</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -6674,56 +6683,56 @@
         <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C17" s="1">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D17" s="1">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="4"/>
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" si="6"/>
-        <v>92</v>
+        <v>92.2</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="7"/>
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
     </row>
     <row r="20" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -6763,10 +6772,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
@@ -6782,15 +6791,15 @@
       </c>
       <c r="I21" s="1">
         <f>MIN(B21:F21)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" s="1">
         <f>MAX(B21:F21)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K21" s="1">
         <f>AVERAGE(B21:F21)</f>
-        <v>4.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="L21" s="1">
         <f>MEDIAN(B21:F21)</f>
@@ -6801,39 +6810,39 @@
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1">
-        <v>4.4812917709350503E-2</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0.20936107635498</v>
-      </c>
-      <c r="D22" s="9">
-        <v>0.231359958648681</v>
-      </c>
-      <c r="E22" s="9">
-        <v>9.7274303436279297E-2</v>
-      </c>
-      <c r="F22" s="9">
-        <v>3.3207178115844699E-2</v>
+      <c r="B22" s="10">
+        <v>6.3190460205078099E-3</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.92105865478515603</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1.29919052124023E-2</v>
+      </c>
+      <c r="E22" s="10">
+        <v>2.6300191879272398E-2</v>
+      </c>
+      <c r="F22" s="10">
+        <v>5.0382852554321199E-2</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" ref="I22:I25" si="8">MIN(B22:F22)</f>
-        <v>3.3207178115844699E-2</v>
+        <v>6.3190460205078099E-3</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" ref="J22:J25" si="9">MAX(B22:F22)</f>
-        <v>0.231359958648681</v>
+        <v>0.92105865478515603</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" ref="K22:K25" si="10">AVERAGE(B22:F22)</f>
-        <v>0.1232030868530271</v>
+        <v>0.20341053009033194</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" ref="L22:L25" si="11">MEDIAN(B22:F22)</f>
-        <v>9.7274303436279297E-2</v>
+        <v>2.6300191879272398E-2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -6841,38 +6850,38 @@
         <v>4</v>
       </c>
       <c r="B23" s="1">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C23" s="1">
-        <v>31</v>
+        <v>19893</v>
       </c>
       <c r="D23" s="1">
-        <v>31</v>
+        <v>154</v>
       </c>
       <c r="E23" s="1">
-        <v>31</v>
+        <v>274</v>
       </c>
       <c r="F23" s="1">
-        <v>71</v>
+        <v>589</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="9"/>
-        <v>71</v>
+        <v>19893</v>
       </c>
       <c r="K23" s="1">
         <f t="shared" si="10"/>
-        <v>39</v>
+        <v>4207.6000000000004</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>274</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -6880,38 +6889,38 @@
         <v>3</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>16925</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="F24" s="1">
-        <v>41</v>
+        <v>467</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="9"/>
-        <v>41</v>
+        <v>16925</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="10"/>
-        <v>8.1999999999999993</v>
+        <v>3551.8</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -6919,16 +6928,16 @@
         <v>10</v>
       </c>
       <c r="B25" s="1">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1">
+        <v>148</v>
+      </c>
+      <c r="D25" s="1">
         <v>142</v>
       </c>
-      <c r="C25" s="1">
-        <v>123</v>
-      </c>
-      <c r="D25" s="1">
-        <v>120</v>
-      </c>
       <c r="E25" s="1">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F25" s="1">
         <v>139</v>
@@ -6938,15 +6947,15 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" si="8"/>
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="9"/>
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="10"/>
-        <v>133</v>
+        <v>134.6</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="11"/>
@@ -6955,20 +6964,20 @@
     </row>
     <row r="26" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
     </row>
     <row r="28" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -7011,7 +7020,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1">
         <v>6</v>
@@ -7031,11 +7040,11 @@
       </c>
       <c r="J29" s="1">
         <f>MAX(B29:F29)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K29" s="1">
         <f>AVERAGE(B29:F29)</f>
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="L29" s="1">
         <f>MEDIAN(B29:F29)</f>
@@ -7046,39 +7055,39 @@
       <c r="A30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="1">
-        <v>0.69834780693054199</v>
-      </c>
-      <c r="C30" s="9">
-        <v>32.137259006500202</v>
-      </c>
-      <c r="D30" s="9">
-        <v>0.82529377937316895</v>
-      </c>
-      <c r="E30" s="9">
-        <v>0.296684980392456</v>
-      </c>
-      <c r="F30" s="9">
-        <v>0.25186681747436501</v>
+      <c r="B30" s="10">
+        <v>0.131369829177856</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1.0380160808563199</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0.35393095016479398</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0.83887100219726496</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.30499982833862299</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" ref="I30:I33" si="12">MIN(B30:F30)</f>
-        <v>0.25186681747436501</v>
+        <v>0.131369829177856</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" ref="J30:J33" si="13">MAX(B30:F30)</f>
-        <v>32.137259006500202</v>
+        <v>1.0380160808563199</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" ref="K30:K33" si="14">AVERAGE(B30:F30)</f>
-        <v>6.8418904781341467</v>
+        <v>0.53343753814697159</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" ref="L30:L33" si="15">MEDIAN(B30:F30)</f>
-        <v>0.69834780693054199</v>
+        <v>0.35393095016479398</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -7086,38 +7095,38 @@
         <v>4</v>
       </c>
       <c r="B31" s="1">
-        <v>326</v>
-      </c>
-      <c r="C31" s="1">
-        <v>35</v>
+        <v>2551</v>
+      </c>
+      <c r="C31" s="10">
+        <v>16933</v>
       </c>
       <c r="D31" s="1">
-        <v>65</v>
+        <v>5389</v>
       </c>
       <c r="E31" s="1">
-        <v>92</v>
+        <v>14950</v>
       </c>
       <c r="F31" s="1">
-        <v>122</v>
+        <v>4407</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="12"/>
-        <v>35</v>
+        <v>2551</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="13"/>
-        <v>326</v>
+        <v>16933</v>
       </c>
       <c r="K31" s="1">
         <f t="shared" si="14"/>
-        <v>128</v>
+        <v>8846</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="15"/>
-        <v>92</v>
+        <v>5389</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -7125,38 +7134,38 @@
         <v>3</v>
       </c>
       <c r="B32" s="1">
-        <v>251</v>
+        <v>2026</v>
       </c>
       <c r="C32" s="1">
-        <v>3</v>
+        <v>14678</v>
       </c>
       <c r="D32" s="1">
-        <v>29</v>
+        <v>4434</v>
       </c>
       <c r="E32" s="1">
-        <v>51</v>
+        <v>12028</v>
       </c>
       <c r="F32" s="1">
-        <v>75</v>
+        <v>3654</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>2026</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="13"/>
-        <v>251</v>
+        <v>14678</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="14"/>
-        <v>81.8</v>
+        <v>7364</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="15"/>
-        <v>51</v>
+        <v>4434</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -7164,34 +7173,34 @@
         <v>10</v>
       </c>
       <c r="B33" s="1">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="C33" s="1">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="D33" s="1">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E33" s="1">
         <v>186</v>
       </c>
       <c r="F33" s="1">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" si="12"/>
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="13"/>
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" si="14"/>
-        <v>186.8</v>
+        <v>182.2</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="15"/>
@@ -7200,20 +7209,20 @@
     </row>
     <row r="34" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
     </row>
     <row r="36" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -7265,7 +7274,7 @@
         <v>7</v>
       </c>
       <c r="F37" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>9</v>
@@ -7276,11 +7285,11 @@
       </c>
       <c r="J37" s="1">
         <f>MAX(B37:F37)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K37" s="1">
         <f>AVERAGE(B37:F37)</f>
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="L37" s="1">
         <f>MEDIAN(B37:F37)</f>
@@ -7291,39 +7300,39 @@
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="1">
-        <v>2.79898905754089</v>
-      </c>
-      <c r="C38" s="9">
-        <v>2.29341387748718</v>
-      </c>
-      <c r="D38" s="9">
-        <v>6.1983330249786297</v>
-      </c>
-      <c r="E38" s="9">
-        <v>1.60025405883789</v>
-      </c>
-      <c r="F38" s="9">
-        <v>280.08687400817797</v>
+      <c r="B38" s="10">
+        <v>4.6643912792205802</v>
+      </c>
+      <c r="C38" s="10">
+        <v>2.0657799243927002</v>
+      </c>
+      <c r="D38" s="11">
+        <v>4.9732720851898096</v>
+      </c>
+      <c r="E38" s="10">
+        <v>0.85173106193542403</v>
+      </c>
+      <c r="F38" s="10">
+        <v>7.9749341011047301</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" ref="I38:I41" si="16">MIN(B38:F38)</f>
-        <v>1.60025405883789</v>
+        <v>0.85173106193542403</v>
       </c>
       <c r="J38" s="1">
         <f t="shared" ref="J38:J41" si="17">MAX(B38:F38)</f>
-        <v>280.08687400817797</v>
+        <v>7.9749341011047301</v>
       </c>
       <c r="K38" s="1">
         <f t="shared" ref="K38:K41" si="18">AVERAGE(B38:F38)</f>
-        <v>58.595572805404515</v>
+        <v>4.1060216903686486</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" ref="L38:L41" si="19">MEDIAN(B38:F38)</f>
-        <v>2.79898905754089</v>
+        <v>4.6643912792205802</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -7331,38 +7340,38 @@
         <v>4</v>
       </c>
       <c r="B39" s="1">
-        <v>31</v>
-      </c>
-      <c r="C39" s="1">
-        <v>332</v>
+        <v>80567</v>
+      </c>
+      <c r="C39" s="10">
+        <v>39302</v>
       </c>
       <c r="D39" s="1">
-        <v>86</v>
+        <v>54602</v>
       </c>
       <c r="E39" s="1">
-        <v>42</v>
+        <v>12545</v>
       </c>
       <c r="F39" s="1">
-        <v>57</v>
+        <v>69103</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" si="16"/>
-        <v>31</v>
+        <v>12545</v>
       </c>
       <c r="J39" s="1">
         <f t="shared" si="17"/>
-        <v>332</v>
+        <v>80567</v>
       </c>
       <c r="K39" s="1">
         <f t="shared" si="18"/>
-        <v>109.6</v>
+        <v>51223.8</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="19"/>
-        <v>57</v>
+        <v>54602</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -7370,38 +7379,38 @@
         <v>3</v>
       </c>
       <c r="B40" s="1">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1">
-        <v>260</v>
+        <v>67853</v>
+      </c>
+      <c r="C40" s="10">
+        <v>33346</v>
       </c>
       <c r="D40" s="1">
-        <v>45</v>
+        <v>43640</v>
       </c>
       <c r="E40" s="1">
-        <v>9</v>
+        <v>10644</v>
       </c>
       <c r="F40" s="1">
-        <v>22</v>
+        <v>57126</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10644</v>
       </c>
       <c r="J40" s="1">
         <f t="shared" si="17"/>
-        <v>260</v>
+        <v>67853</v>
       </c>
       <c r="K40" s="1">
         <f t="shared" si="18"/>
-        <v>67.2</v>
+        <v>42521.8</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" si="19"/>
-        <v>22</v>
+        <v>43640</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -7409,56 +7418,56 @@
         <v>10</v>
       </c>
       <c r="B41" s="1">
+        <v>230</v>
+      </c>
+      <c r="C41" s="1">
+        <v>236</v>
+      </c>
+      <c r="D41" s="1">
+        <v>228</v>
+      </c>
+      <c r="E41" s="1">
+        <v>231</v>
+      </c>
+      <c r="F41" s="8">
         <v>229</v>
-      </c>
-      <c r="C41" s="1">
-        <v>229</v>
-      </c>
-      <c r="D41" s="1">
-        <v>227</v>
-      </c>
-      <c r="E41" s="1">
-        <v>244</v>
-      </c>
-      <c r="F41" s="8">
-        <v>244</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I41" s="1">
         <f t="shared" si="16"/>
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J41" s="1">
         <f t="shared" si="17"/>
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="K41" s="1">
         <f t="shared" si="18"/>
-        <v>234.6</v>
+        <v>230.8</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="19"/>
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
     </row>
     <row r="44" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -7536,39 +7545,39 @@
       <c r="A46" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="1">
-        <v>9.7150390148162806</v>
-      </c>
-      <c r="C46" s="9">
-        <v>598.32735085487298</v>
-      </c>
-      <c r="D46" s="9">
-        <v>315.32704210281298</v>
-      </c>
-      <c r="E46" s="9">
-        <v>265.21624302864001</v>
-      </c>
-      <c r="F46" s="9">
-        <v>1425.36915469169</v>
+      <c r="B46" s="10">
+        <v>25.7871830463409</v>
+      </c>
+      <c r="C46" s="10">
+        <v>377.88461303710898</v>
+      </c>
+      <c r="D46" s="10">
+        <v>109.210680007934</v>
+      </c>
+      <c r="E46" s="10">
+        <v>1760.6418681144701</v>
+      </c>
+      <c r="F46" s="10">
+        <v>277.79642701148902</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" ref="I46:I49" si="20">MIN(B46:F46)</f>
-        <v>9.7150390148162806</v>
+        <v>25.7871830463409</v>
       </c>
       <c r="J46" s="1">
         <f t="shared" ref="J46:J49" si="21">MAX(B46:F46)</f>
-        <v>1425.36915469169</v>
+        <v>1760.6418681144701</v>
       </c>
       <c r="K46" s="1">
         <f t="shared" ref="K46:K49" si="22">AVERAGE(B46:F46)</f>
-        <v>522.7909659385665</v>
+        <v>510.26415424346862</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" ref="L46:L49" si="23">MEDIAN(B46:F46)</f>
-        <v>315.32704210281298</v>
+        <v>277.79642701148902</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -7576,38 +7585,38 @@
         <v>4</v>
       </c>
       <c r="B47" s="1">
-        <v>82</v>
-      </c>
-      <c r="C47" s="1">
-        <v>93</v>
-      </c>
-      <c r="D47" s="1">
-        <v>5326</v>
-      </c>
-      <c r="E47" s="1">
-        <v>21</v>
+        <v>456827</v>
+      </c>
+      <c r="C47" s="10">
+        <v>5594237</v>
+      </c>
+      <c r="D47" s="10">
+        <v>1380314</v>
+      </c>
+      <c r="E47" s="10">
+        <v>29281831</v>
       </c>
       <c r="F47" s="1">
-        <v>35</v>
+        <v>2980276</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="20"/>
-        <v>21</v>
+        <v>456827</v>
       </c>
       <c r="J47" s="1">
         <f t="shared" si="21"/>
-        <v>5326</v>
+        <v>29281831</v>
       </c>
       <c r="K47" s="1">
         <f t="shared" si="22"/>
-        <v>1111.4000000000001</v>
+        <v>7938697</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="23"/>
-        <v>82</v>
+        <v>2980276</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -7615,38 +7624,38 @@
         <v>3</v>
       </c>
       <c r="B48" s="1">
-        <v>46</v>
-      </c>
-      <c r="C48" s="1">
-        <v>50</v>
-      </c>
-      <c r="D48" s="1">
-        <v>4277</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
+        <v>376609</v>
+      </c>
+      <c r="C48" s="10">
+        <v>4666384</v>
+      </c>
+      <c r="D48" s="10">
+        <v>1099275</v>
+      </c>
+      <c r="E48" s="10">
+        <v>24789700</v>
       </c>
       <c r="F48" s="1">
-        <v>3</v>
+        <v>2406045</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>376609</v>
       </c>
       <c r="J48" s="1">
         <f t="shared" si="21"/>
-        <v>4277</v>
+        <v>24789700</v>
       </c>
       <c r="K48" s="1">
         <f t="shared" si="22"/>
-        <v>875.2</v>
+        <v>6667602.5999999996</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" si="23"/>
-        <v>46</v>
+        <v>2406045</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -7654,152 +7663,157 @@
         <v>10</v>
       </c>
       <c r="B49" s="1">
-        <v>283</v>
-      </c>
-      <c r="C49" s="1">
-        <v>281</v>
-      </c>
-      <c r="D49" s="1">
-        <v>281</v>
+        <v>275</v>
+      </c>
+      <c r="C49" s="10">
+        <v>291</v>
+      </c>
+      <c r="D49" s="10">
+        <v>297</v>
       </c>
       <c r="E49" s="1">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F49" s="1">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" si="20"/>
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J49" s="1">
         <f t="shared" si="21"/>
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="K49" s="1">
         <f t="shared" si="22"/>
-        <v>281.8</v>
+        <v>287.8</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" si="23"/>
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="65" spans="10:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="J65" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
+      <c r="J65" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
     </row>
     <row r="66" spans="10:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J66" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
-      <c r="M66" s="16"/>
+      <c r="J66" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
+      <c r="M66" s="13"/>
     </row>
     <row r="67" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
-      <c r="M67" s="16"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
     </row>
     <row r="68" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J68" s="16"/>
-      <c r="K68" s="16"/>
-      <c r="L68" s="16"/>
-      <c r="M68" s="16"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="13"/>
     </row>
     <row r="69" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J69" s="16"/>
-      <c r="K69" s="16"/>
-      <c r="L69" s="16"/>
-      <c r="M69" s="16"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="13"/>
     </row>
     <row r="70" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
-      <c r="L70" s="16"/>
-      <c r="M70" s="16"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
     </row>
     <row r="71" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
-      <c r="M71" s="16"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
     </row>
     <row r="72" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J72" s="16"/>
-      <c r="K72" s="16"/>
-      <c r="L72" s="16"/>
-      <c r="M72" s="16"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="13"/>
     </row>
     <row r="73" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="16"/>
-      <c r="M73" s="16"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
     </row>
     <row r="74" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-      <c r="L74" s="16"/>
-      <c r="M74" s="16"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
     </row>
     <row r="75" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J75" s="10"/>
-      <c r="K75" s="10"/>
-      <c r="L75" s="10"/>
-      <c r="M75" s="10"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
     </row>
     <row r="76" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J76" s="10"/>
-      <c r="K76" s="10"/>
-      <c r="L76" s="10"/>
-      <c r="M76" s="10"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
     </row>
     <row r="77" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J77" s="10"/>
-      <c r="K77" s="10"/>
-      <c r="L77" s="10"/>
-      <c r="M77" s="10"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
     </row>
     <row r="78" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
     </row>
     <row r="79" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J79" s="10"/>
-      <c r="K79" s="10"/>
-      <c r="L79" s="10"/>
-      <c r="M79" s="10"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
+      <c r="M79" s="13"/>
+    </row>
+    <row r="80" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
+      <c r="M80" s="13"/>
     </row>
     <row r="81" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-      <c r="K81" s="14"/>
-      <c r="L81" s="14"/>
-      <c r="M81" s="14"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="12"/>
+      <c r="M81" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B81:M81"/>
-    <mergeCell ref="J66:M74"/>
+  <mergeCells count="10">
+    <mergeCell ref="J66:M80"/>
     <mergeCell ref="J65:M65"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>

</xml_diff>

<commit_message>
fixed q4 with n=105, finished data collection
</commit_message>
<xml_diff>
--- a/a2_q3.xlsx
+++ b/a2_q3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CurtisLui/Documents/Documents/SFU /4th Year/SUMMER 2020/CMPT 310/aima-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F62E17-2C05-9847-A537-C2DCBE5ECB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8799AA4-D9BA-F34E-8B54-8A84C10A200E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="37900" windowHeight="21140" xr2:uid="{1288A5A1-1CE0-7045-B338-BAE7755F7C25}"/>
   </bookViews>
@@ -6182,8 +6182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFCA1D8-37C5-FA4D-BDD1-DACA3CAE6D4E}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added more info into q3
</commit_message>
<xml_diff>
--- a/a2_q3.xlsx
+++ b/a2_q3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CurtisLui/Documents/Documents/SFU /4th Year/SUMMER 2020/CMPT 310/aima-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8799AA4-D9BA-F34E-8B54-8A84C10A200E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ADEC0A-66AB-924E-83EE-687AB24EE816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="37900" windowHeight="21140" xr2:uid="{1288A5A1-1CE0-7045-B338-BAE7755F7C25}"/>
+    <workbookView xWindow="12820" yWindow="0" windowWidth="25580" windowHeight="21600" xr2:uid="{1288A5A1-1CE0-7045-B338-BAE7755F7C25}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Friendship Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
   <si>
     <t>rand_graph(0.1, 31)</t>
   </si>
@@ -93,15 +94,215 @@
     <t>Result Discussion</t>
   </si>
   <si>
-    <t>From the graphs above, we can see that the number of CSP variables assigned and unassigned are strongly correlated. When the number of assigned variables increases, the number of unassigned variables increases. This verifies that our backtracking search is working correctly because when backtracking it will unassign variables, thus increasing the number of times we need to assign variables in order to reach the final solution.
-We can also see that the number of variables assigned and unassigned is proportional to the running time of the algorithm. This means that the longer backtracking search is running, the more CSP variables are being assigned and unassigned.</t>
+    <t>Initial Graph</t>
+  </si>
+  <si>
+    <t>{0: [21, 24], 1: [3, 7, 11, 17, 29], 2: [4, 7, 10, 20, 21], 3: [1, 25, 27], 4: [2, 29], 5: [28], 6: [8, 9, 17, 22], 7: [1, 2, 19, 22], 8: [6, 19], 9: [6, 30], 10: [2, 12, 17], 11: [1], 12: [10, 20, 25], 13: [17, 30], 14: [16, 28], 15: [16, 23], 16: [14, 15, 29], 17: [1, 6, 10, 13, 23], 18: [22, 28], 19: [7, 8, 23], 20: [2, 12], 21: [0, 2, 23], 22: [6, 7, 18], 23: [15, 17, 19, 21], 24: [0], 25: [3, 12], 26: [], 27: [3, 29], 28: [5, 14, 18], 29: [1, 4, 16, 27], 30: [9, 13]}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From the graphs above, we can see that the number of CSP variables assigned and unassigned are strongly correlated. When the number of assigned variables increases, the number of unassigned variables increases. This verifies that our backtracking search is working correctly because when backtracking it will unassign variables, thus increasing the number of times we need to assign variables in order to reach the final solution.
+We can also see that the number of variables assigned and unassigned is proportional to the running time of the algorithm. This means that the longer backtracking search is running, the more CSP variables are being assigned and unassigned.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: There is an additional sheet (Friendship Graphs) that contains the initial friendship graphs for the above results</t>
+    </r>
+  </si>
+  <si>
+    <t>{0: [9, 16, 20], 1: [2, 19, 22, 23, 28], 2: [1, 22], 3: [11, 16, 26], 4: [9, 10, 14, 27], 5: [7, 8, 13], 6: [16, 29], 7: [5, 9, 13, 21, 24, 25], 8: [5, 28], 9: [0, 4, 7, 22, 27], 10: [4, 13, 20], 11: [3, 12, 29], 12: [11], 13: [5, 7, 10, 17], 14: [4, 24], 15: [26], 16: [0, 3, 6], 17: [13, 23, 26], 18: [], 19: [1, 21, 27], 20: [0, 10, 27], 21: [7, 19, 25], 22: [1, 2, 9, 28], 23: [1, 17, 26, 29], 24: [7, 14], 25: [7, 21], 26: [3, 15, 17, 23, 27], 27: [4, 9, 19, 20, 26], 28: [1, 8, 22], 29: [6, 11, 23], 30: []}</t>
+  </si>
+  <si>
+    <t>{0: [4, 5, 7, 17, 24, 27], 1: [14, 20, 24, 26, 29], 2: [5, 9, 12, 13, 14, 15, 16, 17], 3: [11, 12, 13, 27, 28], 4: [0, 9, 14, 17, 24], 5: [0, 2, 9, 12, 18, 21, 23], 6: [7, 22], 7: [0, 6, 10, 12, 26, 27, 30], 8: [12, 13, 18, 19, 20, 21, 28], 9: [2, 4, 5, 12, 17, 18, 21, 28, 30], 10: [7, 20, 22], 11: [3, 22], 12: [2, 3, 5, 7, 8, 9, 14, 19, 26, 27], 13: [2, 3, 8, 14, 20, 21, 24, 25, 27], 14: [1, 2, 4, 12, 13, 19, 22, 25, 26], 15: [2, 21, 23, 24, 27], 16: [2, 19, 25, 27, 30], 17: [0, 2, 4, 9, 25], 18: [5, 8, 9, 19, 21, 22, 23, 25], 19: [8, 12, 14, 16, 18, 27], 20: [1, 8, 10, 13, 24], 21: [5, 8, 9, 13, 15, 18, 25, 27], 22: [6, 10, 11, 14, 18, 24, 28], 23: [5, 15, 18, 26, 27, 29, 30], 24: [0, 1, 4, 13, 15, 20, 22], 25: [13, 14, 16, 17, 18, 21], 26: [1, 7, 12, 14, 23], 27: [0, 3, 7, 12, 13, 15, 16, 19, 21, 23], 28: [3, 8, 9, 22, 30], 29: [1, 23], 30: [7, 9, 16, 23, 28]}</t>
+  </si>
+  <si>
+    <t>{0: [3, 9, 15, 16, 20, 21, 22, 24, 28], 1: [3, 5, 16, 17, 18, 19, 24, 28], 2: [4, 5, 7, 12, 13, 15, 23, 24, 27], 3: [0, 1, 6, 7, 11, 18, 21, 22, 23, 25, 27, 28], 4: [2, 9, 10, 11, 12, 22, 26, 27, 28], 5: [1, 2, 14, 16, 20, 22, 24, 25], 6: [3, 9, 15, 22, 23, 25], 7: [2, 3, 11, 14, 23, 27, 28, 29], 8: [17, 21, 22, 28, 30], 9: [0, 4, 6, 10, 11, 12, 14, 15, 18, 19, 21, 26, 29, 30], 10: [4, 9, 15, 16, 17, 18, 19, 25, 28, 29], 11: [3, 4, 7, 9, 14, 16, 20, 27, 28], 12: [2, 4, 9, 14, 16, 24, 30], 13: [2, 15, 17, 21, 23, 29], 14: [5, 7, 9, 11, 12, 19, 20, 21, 28, 29], 15: [0, 2, 6, 9, 10, 13, 19, 20, 22, 28, 30], 16: [0, 1, 5, 10, 11, 12, 22, 29], 17: [1, 8, 10, 13, 20, 22, 23, 28], 18: [1, 3, 9, 10, 20, 21, 24, 25, 26, 28, 29, 30], 19: [1, 9, 10, 14, 15, 23, 24, 27, 28], 20: [0, 5, 11, 14, 15, 17, 18, 23, 30], 21: [0, 3, 8, 9, 13, 14, 18, 29], 22: [0, 3, 4, 5, 6, 8, 15, 16, 17, 24, 27], 23: [2, 3, 6, 7, 13, 17, 19, 20, 24], 24: [0, 1, 2, 5, 12, 18, 19, 22, 23, 26, 28, 29], 25: [3, 5, 6, 10, 18, 26, 29], 26: [4, 9, 18, 24, 25], 27: [2, 3, 4, 7, 11, 19, 22, 28], 28: [0, 1, 3, 4, 7, 8, 10, 11, 14, 15, 17, 18, 19, 24, 27], 29: [7, 9, 10, 13, 14, 16, 18, 21, 24, 25, 30], 30: [8, 9, 12, 15, 18, 20, 29]}</t>
+  </si>
+  <si>
+    <t>{0: [1, 3, 5, 6, 7, 9, 11, 12, 15, 16, 17, 18, 20, 21, 23, 30], 1: [0, 3, 4, 6, 7, 8, 9, 11, 12, 15, 16, 19, 26, 29, 30], 2: [6, 7, 9, 13, 14, 15, 18, 19, 24, 26, 27], 3: [0, 1, 6, 7, 8, 13, 15, 16, 17, 21, 22], 4: [1, 5, 6, 9, 11, 13, 15, 16, 18, 19, 20, 22, 26, 27, 28, 29, 30], 5: [0, 4, 6, 8, 11, 12, 13, 14, 15, 18, 19, 21, 24, 25, 27, 29], 6: [0, 1, 2, 3, 4, 5, 10, 12, 15, 17, 18, 26, 29, 30], 7: [0, 1, 2, 3, 11, 14, 17, 18, 20, 21, 22, 24, 26, 27, 29], 8: [1, 3, 5, 11, 13, 14, 17, 18, 19, 25, 26, 29], 9: [0, 1, 2, 4, 10, 13, 19, 20, 22, 23, 26], 10: [6, 9, 12, 14, 16, 17, 22, 27, 29], 11: [0, 1, 4, 5, 7, 8, 15, 17, 19, 21, 22, 23, 25, 26, 28, 29], 12: [0, 1, 5, 6, 10, 14, 16, 20, 21, 23, 24, 26, 28, 30], 13: [2, 3, 4, 5, 8, 9, 14, 18, 19, 20, 22, 26, 27], 14: [2, 5, 7, 8, 10, 12, 13, 16, 18, 19, 20, 23, 24, 28, 30], 15: [0, 1, 2, 3, 4, 5, 6, 11, 16, 22, 24, 25, 26, 29], 16: [0, 1, 3, 4, 10, 12, 14, 15, 17, 19, 20, 21, 22, 25, 26, 29], 17: [0, 3, 6, 7, 8, 10, 11, 16, 21, 22, 26, 30], 18: [0, 2, 4, 5, 6, 7, 8, 13, 14, 19, 21, 22, 24, 29], 19: [1, 2, 4, 5, 8, 9, 11, 13, 14, 16, 18, 24, 25, 26, 27], 20: [0, 4, 7, 9, 12, 13, 14, 16, 24, 26, 28], 21: [0, 3, 5, 7, 11, 12, 16, 17, 18, 22, 25], 22: [3, 4, 7, 9, 10, 11, 13, 15, 16, 17, 18, 21, 25, 27, 28, 30], 23: [0, 9, 11, 12, 14, 24, 25, 26, 30], 24: [2, 5, 7, 12, 14, 15, 18, 19, 20, 23, 25, 26, 29], 25: [5, 8, 11, 15, 16, 19, 21, 22, 23, 24, 26, 27, 29], 26: [1, 2, 4, 6, 7, 8, 9, 11, 12, 13, 15, 16, 17, 19, 20, 23, 24, 25, 28, 29, 30], 27: [2, 4, 5, 7, 10, 13, 19, 22, 25, 28], 28: [4, 11, 12, 14, 20, 22, 26, 27, 29], 29: [1, 4, 5, 6, 7, 8, 10, 11, 15, 16, 18, 24, 25, 26, 28, 30], 30: [0, 1, 4, 6, 12, 14, 17, 22, 23, 26, 29]}</t>
+  </si>
+  <si>
+    <t>{0: [3, 4, 5, 6, 7, 14, 15, 16, 21, 23, 24, 26, 27, 28], 1: [2, 3, 4, 5, 7, 11, 12, 13, 15, 16, 21, 22, 24, 27], 2: [1, 6, 8, 11, 13, 15, 16, 18, 21, 23, 27, 28, 29, 30], 3: [0, 1, 5, 9, 10, 11, 15, 19, 22, 24, 25, 27, 28, 30], 4: [0, 1, 8, 9, 13, 14, 16, 19, 22, 23, 24, 25, 26], 5: [0, 1, 3, 7, 8, 10, 11, 12, 13, 17, 21, 23, 25, 26, 28, 29], 6: [0, 2, 10, 11, 12, 14, 15, 17, 18, 21, 22, 25, 27, 29, 30], 7: [0, 1, 5, 10, 12, 14, 15, 16, 17, 19, 20, 22, 25, 26, 27, 29, 30], 8: [2, 4, 5, 9, 13, 15, 17, 19, 21, 22, 23, 26, 30], 9: [3, 4, 8, 10, 11, 13, 14, 15, 18, 19, 23, 24, 25, 27, 29, 30], 10: [3, 5, 6, 7, 9, 12, 13, 14, 15, 18, 19, 20, 21, 23, 24, 26, 28], 11: [1, 2, 3, 5, 6, 9, 15, 16, 17, 21, 22, 25, 26, 27, 29], 12: [1, 5, 6, 7, 10, 13, 14, 16, 22, 24, 25, 27, 28], 13: [1, 2, 4, 5, 8, 9, 10, 12, 15, 16, 19, 23, 26], 14: [0, 4, 6, 7, 9, 10, 12, 15, 16, 17, 21, 22, 28, 30], 15: [0, 1, 2, 3, 6, 7, 8, 9, 10, 11, 13, 14, 17, 19, 20, 22, 23, 24, 27, 28, 29, 30], 16: [0, 1, 2, 4, 7, 11, 12, 13, 14, 17, 19, 20, 22, 23, 24, 26, 28, 30], 17: [5, 6, 7, 8, 11, 14, 15, 16, 18, 19, 20, 21, 26, 27, 30], 18: [2, 6, 9, 10, 17, 19, 20, 22, 25, 26, 28, 30], 19: [3, 4, 7, 8, 9, 10, 13, 15, 16, 17, 18, 20, 21, 24, 25, 26, 29], 20: [7, 10, 15, 16, 17, 18, 19, 23, 24, 26, 27], 21: [0, 1, 2, 5, 6, 8, 10, 11, 14, 17, 19, 22, 23, 24, 26, 27, 29, 30], 22: [1, 3, 4, 6, 7, 8, 11, 12, 14, 15, 16, 18, 21, 23, 24, 25, 26, 27], 23: [0, 2, 4, 5, 8, 9, 10, 13, 15, 16, 20, 21, 22, 24, 26, 28, 29], 24: [0, 1, 3, 4, 9, 10, 12, 15, 16, 19, 20, 21, 22, 23, 26, 27, 28, 30], 25: [3, 4, 5, 6, 7, 9, 11, 12, 18, 19, 22, 27, 28], 26: [0, 4, 5, 7, 8, 10, 11, 13, 16, 17, 18, 19, 20, 21, 22, 23, 24, 27, 28], 27: [0, 1, 2, 3, 6, 7, 9, 11, 12, 15, 17, 20, 21, 22, 24, 25, 26, 29], 28: [0, 2, 3, 5, 10, 12, 14, 15, 16, 18, 23, 24, 25, 26, 29, 30], 29: [2, 5, 6, 7, 9, 11, 15, 19, 21, 23, 27, 28, 30], 30: [2, 3, 6, 7, 8, 9, 14, 15, 16, 17, 18, 21, 24, 28, 29]}</t>
+  </si>
+  <si>
+    <t>{0: [1, 2, 3, 5, 6, 7, 9, 10, 11, 14, 15, 16, 17, 18, 22, 23, 24, 25, 27, 29, 30], 1: [0, 6, 7, 8, 9, 10, 14, 15, 17, 20, 22, 23, 24, 25, 26, 27, 28, 30], 2: [0, 3, 4, 5, 6, 8, 10, 13, 14, 15, 17, 18, 20, 23, 25, 27], 3: [0, 2, 8, 9, 11, 12, 13, 20, 21, 22, 23, 25, 26], 4: [2, 9, 10, 11, 14, 16, 17, 18, 19, 21, 22, 24, 25, 26, 27, 29], 5: [0, 2, 6, 9, 10, 12, 13, 17, 19, 23, 24, 25, 27, 28, 30], 6: [0, 1, 2, 5, 9, 10, 15, 16, 17, 19, 20, 21, 22, 23, 24, 25, 28, 29, 30], 7: [0, 1, 8, 9, 10, 13, 14, 15, 16, 17, 19, 21, 22, 23, 25, 26, 27, 30], 8: [1, 2, 3, 7, 9, 10, 11, 14, 16, 17, 18, 19, 20, 22, 23, 25, 28], 9: [0, 1, 3, 4, 5, 6, 7, 8, 14, 16, 18, 19, 20, 21, 22, 25, 26, 27, 28], 10: [0, 1, 2, 4, 5, 6, 7, 8, 12, 13, 14, 17, 20, 21, 22, 25, 27, 29], 11: [0, 3, 4, 8, 12, 21, 22, 23, 25, 27, 29, 30], 12: [3, 5, 10, 11, 13, 14, 16, 17, 19, 20, 21, 22, 24, 26, 27, 29, 30], 13: [2, 3, 5, 7, 10, 12, 14, 15, 16, 17, 19, 20, 21, 23, 24, 27, 28, 30], 14: [0, 1, 2, 4, 7, 8, 9, 10, 12, 13, 15, 16, 17, 18, 20, 21, 22, 24, 26, 27, 29, 30], 15: [0, 1, 2, 6, 7, 13, 14, 16, 17, 18, 19, 20, 21, 22, 23, 27, 28], 16: [0, 4, 6, 7, 8, 9, 12, 13, 14, 15, 19, 20, 21, 22, 24, 26, 27, 28], 17: [0, 1, 2, 4, 5, 6, 7, 8, 10, 12, 13, 14, 15, 18, 19, 20, 22, 24, 25, 27, 28, 29, 30], 18: [0, 2, 4, 8, 9, 14, 15, 17, 19, 22, 23, 24, 26, 29], 19: [4, 5, 6, 7, 8, 9, 12, 13, 15, 16, 17, 18, 20, 21, 22, 23, 24, 25, 27], 20: [1, 2, 3, 6, 8, 9, 10, 12, 13, 14, 15, 16, 17, 19, 21, 24, 25, 27], 21: [3, 4, 6, 7, 9, 10, 11, 12, 13, 14, 15, 16, 19, 20, 22, 23, 24, 25, 26, 27, 29, 30], 22: [0, 1, 3, 4, 6, 7, 8, 9, 10, 11, 12, 14, 15, 16, 17, 18, 19, 21, 25, 26, 27, 28, 29], 23: [0, 1, 2, 3, 5, 6, 7, 8, 11, 13, 15, 18, 19, 21, 24, 25, 26, 27, 29, 30], 24: [0, 1, 4, 5, 6, 12, 13, 14, 16, 17, 18, 19, 20, 21, 23, 29], 25: [0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 17, 19, 20, 21, 22, 23, 26, 28, 30], 26: [1, 3, 4, 7, 9, 12, 14, 16, 18, 21, 22, 23, 25, 27, 30], 27: [0, 1, 2, 4, 5, 7, 9, 10, 11, 12, 13, 14, 15, 16, 17, 19, 20, 21, 22, 23, 26, 30], 28: [1, 5, 6, 8, 9, 13, 15, 16, 17, 22, 25, 29], 29: [0, 4, 6, 10, 11, 12, 14, 17, 18, 21, 22, 23, 24, 28], 30: [0, 1, 5, 6, 7, 11, 12, 13, 14, 17, 21, 23, 25, 26, 27]}</t>
+  </si>
+  <si>
+    <t>{11: 0, 29: 1, 12: 1, 6: 0, 23: 0, 3: 1, 16: 2, 26: 2, 17: 1, 27: 0, 13: 0, 5: 1, 7: 2, 9: 1, 0: 0, 4: 2, 10: 1, 20: 2, 1: 1, 19: 2, 28: 0, 22: 2, 2: 0, 8: 2, 14: 0, 24: 1, 25: 0, 21: 1, 15: 0, 30: 0, 18: 0}</t>
+  </si>
+  <si>
+    <t>{3: 0, 11: 1, 27: 1, 12: 2, 19: 0, 8: 1, 14: 1, 2: 0, 15: 2, 26: 0, 23: 3, 5: 1, 9: 3, 28: 2, 21: 0, 7: 3, 18: 2, 25: 3, 13: 2, 16: 2, 1: 2, 4: 0, 0: 2, 17: 1, 20: 0, 29: 0, 24: 1, 30: 0, 22: 0, 6: 1, 10: 1}</t>
+  </si>
+  <si>
+    <t>{13: 0, 17: 1, 23: 2, 20: 0, 2: 1, 24: 0, 28: 2, 1: 3, 15: 4, 19: 1, 0: 1, 3: 0, 18: 4, 6: 1, 21: 2, 9: 0, 10: 3, 29: 1, 4: 4, 27: 3, 7: 4, 25: 2, 14: 3, 11: 1, 12: 2, 22: 2, 30: 3, 5: 4, 16: 0, 26: 1, 8: 0}</t>
+  </si>
+  <si>
+    <t>{4: 0, 13: 1, 9: 2, 26: 3, 19: 4, 2: 0, 1: 1, 16: 2, 20: 4, 14: 3, 5: 2, 18: 5, 29: 4, 6: 6, 15: 5, 11: 6, 7: 2, 8: 0, 25: 1, 24: 6, 22: 3, 3: 4, 21: 0, 0: 3, 12: 5, 30: 2, 28: 1, 23: 0, 10: 0, 27: 5, 17: 1}</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>{24: 0, 23: 1, 10: 2, 28: 3, 15: 4, 9: 3, 20: 3, 3: 5, 19: 1, 0: 6, 26: 4, 5: 0, 7: 5, 16: 2, 4: 5, 17: 6, 30: 1, 13: 6, 8: 2, 11: 1, 27: 2, 29: 6, 14: 0, 1: 3, 22: 6, 21: 5, 25: 4, 6: 3, 12: 1, 2: 0, 18: 5}</t>
+  </si>
+  <si>
+    <t>{20: 0, 24: 1, 17: 2, 1: 3, 6: 4, 15: 1, 14: 4, 27: 5, 19: 3, 13: 6, 12: 7, 21: 2, 16: 8, 10: 1, 5: 8, 2: 3, 22: 0, 7: 7, 23: 0, 30: 1, 26: 6, 0: 6, 25: 5, 4: 7, 8: 6, 9: 1, 28: 7, 18: 5, 29: 3, 11: 4, 3: 8}</t>
+  </si>
+  <si>
+    <t>{0: [1, 14, 18, 20, 23], 1: [0, 3, 4, 10, 12, 19, 25], 2: [23], 3: [1, 8, 9, 29], 4: [1, 10], 5: [17, 18, 22], 6: [11], 7: [27], 8: [3, 15, 28], 9: [3, 10, 17, 24], 10: [1, 4, 9, 12, 13, 23, 29], 11: [6, 21, 29], 12: [1, 10], 13: [10, 14, 29], 14: [0, 13, 28], 15: [8, 23, 28], 16: [27], 17: [5, 9, 23], 18: [0, 5, 27], 19: [1, 27], 20: [0, 23], 21: [11, 23], 22: [5, 26], 23: [0, 2, 10, 15, 17, 20, 21, 28], 24: [9, 26], 25: [1, 26], 26: [22, 24, 25, 30], 27: [7, 16, 18, 19], 28: [8, 14, 15, 23, 29, 30], 29: [3, 10, 11, 13, 28], 30: [26, 28]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0: [1, 5, 12, 17, 19, 23], 1: [0, 4, 8, 13, 14, 20, 23], 2: [3, 5, 7, 11, 13, 14, 25, 26, 27], 3: [2, 5, 8, 9, 22, 28], 4: [1, 9], 5: [0, 2, 3, 6, 7, 25, 28], 6: [5, 25, 29, 30], 7: [2, 5, 14, 21, 25, 28], 8: [1, 3, 14, 18, 21, 22, 24, 30], 9: [3, 4, 11, 12, 13, 23, 26], 10: [14, 19], 11: [2, 9, 21, 23, 24, 27, 28], 12: [0, 9, 17, 20, 21, 22, 23, 25, 26, 28], 13: [1, 2, 9, 14, 16, 17, 22], 14: [1, 2, 7, 8, 10, 13, 18, 20, 26, 28], 15: [21, 23, 29], 16: [13, 18, 25], 17: [0, 12, 13, 19, 26, 28], 18: [8, 14, 16, 20, 21], 19: [0, 10, 17, 24], 20: [1, 12, 14, 18, 23], 21: [7, 8, 11, 12, 15, 18, 23, 24, 28], 22: [3, 8, 12, 13, 24, 26], 23: [0, 1, 9, 11, 12, 15, 20, 21, 27], 24: [8, 11, 19, 21, 22, 25, 27, 29], 25: [2, 5, 6, 7, 12, 16, 24, 30], </t>
+  </si>
+  <si>
+    <t>{9: 0, 13: 1, 16: 0, 2: 0, 14: 2, 7: 1, 18: 1, 26: 1, 1: 0, 20: 3, 8: 3, 12: 2, 21: 0, 28: 3, 23: 1, 5: 2, 0: 3, 17: 0, 25: 3, 3: 1, 22: 0, 11: 2, 27: 3, 24: 1, 19: 2, 15: 2, 6: 0, 29: 3, 30: 2, 4: 1, 10: 0}</t>
+  </si>
+  <si>
+    <t>{21: 0, 23: 1, 0: 0, 20: 2, 14: 1, 1: 1, 13: 0, 10: 2, 12: 0, 4: 0, 29: 1, 11: 2, 6: 0, 18: 1, 3: 0, 9: 1, 8: 1, 19: 0, 27: 2, 24: 0, 25: 0, 7: 0, 16: 0, 17: 0, 5: 2, 26: 1, 22: 0, 2: 0, 28: 0, 15: 2, 30: 2}</t>
+  </si>
+  <si>
+    <t>{0: [7, 14, 24, 28], 1: [4, 5, 6, 8, 10, 13, 16, 19, 25], 2: [3, 5, 6, 8, 16, 26, 27, 28, 29], 3: [2, 7, 9, 15, 21, 25, 29], 4: [1, 5, 7, 8, 15, 18, 26, 27], 5: [1, 2, 4, 7, 8, 9, 13, 23, 24], 6: [1, 2, 12, 16, 18, 22, 29], 7: [0, 3, 4, 5, 9, 10, 14, 18, 22, 24, 26, 27, 28, 30], 8: [1, 2, 4, 5, 17, 20, 25, 26, 30], 9: [3, 5, 7, 10, 14, 15, 26, 30], 10: [1, 7, 9, 13, 15, 17, 21, 26, 28], 11: [14, 17, 18, 19, 21, 24], 12: [6, 17, 18, 23, 28], 13: [1, 5, 10, 14, 15, 16, 18, 19, 22, 26], 14: [0, 7, 9, 11, 13, 21, 22, 24], 15: [3, 4, 9, 10, 13, 16, 22, 24, 26, 27, 30], 16: [1, 2, 6, 13, 15, 18, 21, 23, 26, 27, 30], 17: [8, 10, 11, 12, 19, 23, 24, 25], 18: [4, 6, 7, 11, 12, 13, 16, 23, 26, 28, 30], 19: [1, 11, 13, 17, 23, 24, 25, 27, 28], 20: [8, 25], 21: [3, 10, 11, 14, 16, 23, 28], 22: [6, 7, 13, 14, 15, 27, 29], 23: [5, 12, 16, 17, 18, 19, 21, 24, 26, 29], 24: [0, 5, 7, 11, 14, 15, 17, 19, 23, 25, 29, 30], 25: [1, 3, 8, 17, 19, 20, 24, 28], 26: [2, 4, 7, 8, 9, 10, 13, 15, 16, 18, 23, 27], 27: [2, 4, 7, 15, 16, 19, 22, 26], 28: [0, 2, 7, 10, 12, 18, 19, 21, 25], 29: [2, 3, 6, 22, 23, 24], 30: [7, 8, 9, 15, 16, 18, 24]}</t>
+  </si>
+  <si>
+    <t>{24: 0, 23: 1, 19: 2, 17: 3, 25: 1, 11: 1, 14: 2, 21: 0, 28: 3, 7: 1, 0: 4, 10: 2, 22: 0, 27: 4, 16: 2, 26: 0, 2: 1, 18: 4, 30: 3, 6: 3, 9: 4, 15: 1, 13: 3, 5: 2, 8: 4, 1: 0, 4: 3, 29: 2, 3: 3, 12: 2, 20: 0}</t>
+  </si>
+  <si>
+    <t>{0: [1, 2, 3, 4, 7, 8, 10, 11, 15, 18, 20, 23, 24, 25, 27, 28], 1: [0, 5, 7, 9, 11, 15, 16, 18, 21, 22, 29], 2: [0, 4, 6, 7, 8, 10, 12, 13, 18, 19, 23, 27], 3: [0, 5, 6, 10, 13, 14, 19, 25, 26, 27, 28, 30], 4: [0, 2, 5, 6, 8, 10, 11, 13, 16, 18, 23, 26, 28, 29, 30], 5: [1, 3, 4, 8, 11, 13, 17, 23, 25, 28, 30], 6: [2, 3, 4, 11, 14, 15, 18, 20, 22, 24, 25, 28], 7: [0, 1, 2, 8, 9, 11, 20, 25, 29], 8: [0, 2, 4, 5, 7, 9, 12, 15, 16, 18, 24, 29], 9: [1, 7, 8, 10, 11, 13, 14, 19, 21, 23, 26, 27, 30], 10: [0, 2, 3, 4, 9, 12, 15, 19, 21, 22, 23, 27, 28, 29], 11: [0, 1, 4, 5, 6, 7, 9, 13, 19, 20, 23, 24, 25, 26, 28, 29, 30], 12: [2, 8, 10, 20, 21, 22, 23, 24, 27, 29, 30], 13: [2, 3, 4, 5, 9, 11, 17, 20, 21, 22, 25, 26, 27], 14: [3, 6, 9, 16, 24, 26, 29, 30], 15: [0, 1, 6, 8, 10, 16, 17, 18, 20, 24, 27, 28, 29], 16: [1, 4, 8, 14, 15, 18, 22, 23, 25, 27, 29, 30], 17: [5, 13, 15, 20, 22, 25], 18: [0, 1, 2, 4, 6, 8, 15, 16, 19, 22, 24, 26, 27], 19: [2, 3, 9, 10, 11, 18, 20, 22], 20: [0, 6, 7, 11, 12, 13, 15, 17, 19, 21, 26, 27, 28, 30], 21: [1, 9, 10, 12, 13, 20, 22, 24, 25, 27, 30], 22: [1, 6, 10, 12, 13, 16, 17, 18, 19, 21, 24, 25, 28], 23: [0, 2, 4, 5, 9, 10, 11, 12, 16, 24, 27, 28], 24: [0, 6, 8, 11, 12, 14, 15, 18, 21, 22, 23, 25, 30], 25: [0, 3, 5, 6, 7, 11, 13, 16, 17, 21, 22, 24, 26, 28, 30], 26: [3, 4, 9, 11, 13, 14, 18, 20, 25, 27], 27: [0, 2, 3, 9, 10, 12, 13, 15, 16, 18, 20, 21, 23, 26], 28: [0, 3, 4, 5, 6, 10, 11, 15, 20, 22, 23, 25], 29: [1, 4, 7, 8, 10, 11, 12, 14, 15, 16], 30: [3, 4, 5, 9, 11, 12, 14, 16, 20, 21, 24, 25]}</t>
+  </si>
+  <si>
+    <t>{16: 0, 23: 1, 27: 2, 10: 0, 9: 3, 2: 4, 12: 5, 8: 2, 4: 3, 0: 5, 18: 1, 7: 0, 19: 5, 28: 2, 11: 4, 29: 1, 1: 2, 6: 5, 25: 3, 22: 4, 21: 1, 20: 3, 24: 0, 30: 2, 15: 4, 14: 4, 3: 1, 26: 5, 13: 0, 5: 5, 17: 2}</t>
+  </si>
+  <si>
+    <t>{0: [2, 3, 4, 5, 6, 13, 15, 16, 17, 18, 23, 27, 28, 29, 30], 1: [4, 6, 9, 11, 14, 15, 16, 18, 21, 22, 23, 24, 25, 26, 28, 29], 2: [0, 4, 5, 6, 7, 8, 9, 11, 12, 13, 14, 15, 18, 21, 23, 27, 29], 3: [0, 5, 6, 7, 8, 10, 11, 12, 13, 18, 19, 23, 24, 25, 28, 30], 4: [0, 1, 2, 6, 9, 10, 13, 15, 16, 17, 18, 20, 21, 23, 25, 28, 29], 5: [0, 2, 3, 7, 8, 9, 10, 11, 12, 16, 17, 18, 19, 20, 21, 22, 23, 24, 26, 27, 29], 6: [0, 1, 2, 3, 4, 8, 11, 18, 20, 23], 7: [2, 3, 5, 10, 11, 15, 20, 21, 23, 26, 29], 8: [2, 3, 5, 6, 14, 15, 17, 18, 20, 21, 22, 25, 27, 29], 9: [1, 2, 4, 5, 10, 11, 12, 14, 16, 17, 20, 21, 22, 24, 25, 26, 28], 10: [3, 4, 5, 7, 9, 11, 16, 20, 22, 24, 25, 26], 11: [1, 2, 3, 5, 6, 7, 9, 10, 12, 13, 14, 18, 19, 23, 26, 29, 30], 12: [2, 3, 5, 9, 11, 14, 16, 17, 18, 21, 23, 25, 27, 28, 29, 30], 13: [0, 2, 3, 4, 11, 14, 15, 16, 17, 19, 23, 27, 28, 29], 14: [1, 2, 8, 9, 11, 12, 13, 15, 24, 25, 27, 29], 15: [0, 1, 2, 4, 7, 8, 13, 14, 19, 20, 22, 23, 25, 28, 30], 16: [0, 1, 4, 5, 9, 10, 12, 13, 17, 20, 21, 29], 17: [0, 4, 5, 8, 9, 12, 13, 16, 19, 20, 22, 25, 27], 18: [0, 1, 2, 3, 4, 5, 6, 8, 11, 12, 19, 21, 22, 23, 24, 27, 30], 19: [3, 5, 11, 13, 15, 17, 18, 22, 23, 25, 27, 28, 29, 30], 20: [4, 5, 6, 7, 8, 9, 10, 15, 16, 17, 21, 22, 24, 26, 27, 29, 30], 21: [1, 2, 4, 5, 7, 8, 9, 12, 16, 18, 20, 22, 23, 24, 26, 28], 22: [1, 5, 8, 9, 10, 15, 17, 18, 19, 20, 21, 23, 24, 25, 26, 28, 29], 23: [0, 1, 2, 3, 4, 5, 6, 7, 11, 12, 13, 15, 18, 19, 21, 22, 25, 30], 24: [1, 3, 5, 9, 10, 14, 18, 20, 21, 22, 25, 28], 25: [1, 3, 4, 8, 9, 10, 12, 14, 15, 17, 19, 22, 23, 24, 26, 28, 29], 26: [1, 5, 7, 9, 10, 11, 20, 21, 22, 25, 29], 27: [0, 2, 5, 8, 12, 13, 14, 17, 18, 19, 20, 29], 28: [0, 1, 3, 4, 9, 12, 13, 15, 19, 21, 22, 24, 25], 29: [0, 1, 2, 4, 5, 7, 8, 11, 12, 13, 14, 16, 19, 20, 22, 25, 26, 27], 30: [0, 3, 11, 12, 15, 18, 19, 20, 23]}</t>
+  </si>
+  <si>
+    <t>{3: 0, 11: 1, 23: 2, 18: 3, 6: 4, 5: 4, 12: 5, 19: 5, 2: 0, 21: 1, 22: 6, 4: 5, 1: 0, 9: 3, 10: 2, 26: 5, 16: 6, 0: 1, 20: 0, 17: 2, 27: 6, 8: 5, 24: 5, 28: 2, 29: 3, 13: 4, 7: 6, 14: 2, 15: 3, 30: 4, 25: 1}</t>
+  </si>
+  <si>
+    <t>{0: [2, 3, 5, 8, 9, 15, 18, 20, 21, 23, 24, 25, 26, 29, 30], 1: [2, 8, 10, 12, 13, 14, 18, 20, 21, 22, 23, 25, 26, 29, 30], 2: [0, 1, 3, 4, 5, 7, 9, 11, 13, 14, 15, 17, 18, 19, 20, 21, 22, 24, 25, 26, 27, 28, 29], 3: [0, 2, 4, 5, 6, 7, 8, 9, 10, 11, 13, 15, 17, 18, 19, 20, 21, 22, 23, 25, 26, 30], 4: [2, 3, 5, 6, 7, 8, 9, 12, 13, 15, 16, 17, 18, 19, 20, 21, 22, 24, 25, 26, 30], 5: [0, 2, 3, 4, 6, 7, 8, 10, 11, 12, 14, 15, 16, 21, 22, 23, 25, 26, 29, 30], 6: [3, 4, 5, 7, 8, 9, 12, 14, 15, 16, 18, 22, 23, 24, 25, 26, 28, 29], 7: [2, 3, 4, 5, 6, 8, 9, 10, 11, 13, 14, 16, 19, 20, 21, 23, 24, 26, 27, 30], 8: [0, 1, 3, 4, 5, 6, 7, 10, 12, 17, 20, 21, 25, 26, 27, 29, 30], 9: [0, 2, 3, 4, 6, 7, 10, 12, 14, 16, 19, 20, 21, 22, 25, 26, 27, 28, 29], 10: [1, 3, 5, 7, 8, 9, 11, 12, 19, 20, 21, 22, 23, 24, 25, 27, 30], 11: [2, 3, 5, 7, 10, 12, 13, 17, 19, 20, 21, 22, 23, 25, 26, 29, 30], 12: [1, 4, 5, 6, 8, 9, 10, 11, 13, 14, 15, 17, 18, 19, 22, 23, 24, 25, 26, 28, 30], 13: [1, 2, 3, 4, 7, 11, 12, 14, 15, 16, 17, 18, 21, 22, 24, 25, 26, 27, 28, 29, 30], 14: [1, 2, 5, 6, 7, 9, 12, 13, 15, 19, 20, 21, 22, 24, 25, 26, 27, 29, 30], 15: [0, 2, 3, 4, 5, 6, 12, 13, 14, 16, 17, 18, 19, 20, 21, 23, 24, 27, 30], 16: [4, 5, 6, 7, 9, 13, 15, 17, 18, 23, 24, 25, 27, 29], 17: [2, 3, 4, 8, 11, 12, 13, 15, 16, 18, 19, 22, 27, 30], 18: [0, 1, 2, 3, 4, 6, 12, 13, 15, 16, 17, 19, 20, 21, 23, 24, 25, 30], 19: [2, 3, 4, 7, 9, 10, 11, 12, 14, 15, 17, 18, 20, 21, 23, 24, 25, 26, 27, 28, 29], 20: [0, 1, 2, 3, 4, 7, 8, 9, 10, 11, 14, 15, 18, 19, 24, 27, 29], 21: [0, 1, 2, 3, 4, 5, 7, 8, 9, 10, 11, 13, 14, 15, 18, 19, 24, 25, 26, 29], 22: [1, 2, 3, 4, 5, 6, 9, 10, 11, 12, 13, 14, 17, 23, 25, 26, 28, 29], 23: [0, 1, 3, 5, 6, 7, 10, 11, 12, 15, 16, 18, 19, 22, 25, 27, 28, 29, 30], 24: [0, 2, 4, 6, 7, 10, 12, 13, 14, 15, 16, 18, 19, 20, 21, 25, 28, 30], 25: [0, 1, 2, 3, 4, 5, 6, 8, 9, 10, 11, 12, 13, 14, 16, 18, 19, 21, 22, 23, 24, 26, 27, 28, 29, 30], 26: [0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 11, 12, 13, 14, 19, 21, 22, 25, 28, 29, 30], 27: [2, 7, 8, 9, 10, 13, 14, 15, 16, 17, 19, 20, 23, 25, 28, 30], 28: [2, 6, 9, 12, 13, 19, 22, 23, 24, 25, 26, 27, 29, 30], 29: [0, 1, 2, 5, 6, 8, 9, 11, 13, 14, 16, 19, 20, 21, 22, 23, 25, 26, 28, 30], 30: [0, 1, 3, 4, 5, 7, 8, 10, 11, 12, 13, 14, 15, 17, 18, 23, 24, 25, 26, 27, 28, 29]}</t>
+  </si>
+  <si>
+    <t>{6: 0, 12: 1, 14: 2, 26: 3, 22: 4, 5: 5, 25: 6, 9: 5, 28: 2, 23: 7, 29: 1, 11: 2, 3: 1, 2: 7, 4: 2, 13: 0, 1: 5, 21: 4, 18: 3, 16: 4, 30: 4, 24: 5, 8: 7, 7: 6, 19: 0, 10: 3, 20: 4, 15: 6, 17: 5, 27: 1, 0: 0}</t>
+  </si>
+  <si>
+    <t>{0: [20, 26], 1: [27], 2: [9, 21], 3: [19], 4: [12, 17, 22, 23, 24], 5: [7, 15], 6: [8, 26], 7: [5, 17], 8: [6, 10, 15, 27], 9: [2, 13, 18], 10: [8], 11: [17], 12: [4], 13: [9, 19, 28], 14: [28], 15: [5, 8], 16: [19, 26, 28], 17: [4, 7, 11, 27], 18: [9], 19: [3, 13, 16, 22, 26], 20: [0, 21], 21: [2, 20, 27, 29], 22: [4, 19], 23: [4], 24: [4], 25: [], 26: [0, 6, 16, 19], 27: [1, 8, 17, 21], 28: [13, 14, 16, 29], 29: [21, 28], 30: []}</t>
+  </si>
+  <si>
+    <t>{25: 0, 18: 0, 9: 1, 2: 0, 13: 0, 21: 1, 20: 0, 29: 0, 28: 1, 16: 0, 14: 0, 19: 1, 26: 2, 0: 1, 27: 0, 3: 0, 6: 0, 17: 1, 22: 0, 4: 2, 23: 0, 8: 1, 24: 0, 7: 0, 5: 1, 15: 0, 12: 0, 10: 0, 1: 1, 11: 0, 30: 0}</t>
+  </si>
+  <si>
+    <t>{0: [1, 6, 7, 19, 20, 27], 1: [0, 2, 5, 9, 17, 19, 26, 28, 30], 2: [1, 22], 3: [], 4: [7, 12, 13, 16, 18, 25, 29], 5: [1, 19, 22, 29], 6: [0, 12, 20, 21, 27, 28, 30], 7: [0, 4, 13, 19, 20, 26, 30], 8: [13, 19, 22, 28], 9: [1, 12, 29], 10: [13, 24, 26, 29, 30], 11: [20, 21, 23, 26, 28], 12: [4, 6, 9, 16, 17, 28, 29, 30], 13: [4, 7, 8, 10, 15, 16, 24, 28, 30], 14: [18, 25, 27], 15: [13, 16, 19, 24, 27, 28], 16: [4, 12, 13, 15], 17: [1, 12, 28, 29, 30], 18: [4, 14, 26], 19: [0, 1, 5, 7, 8, 15, 25], 20: [0, 6, 7, 11, 23], 21: [6, 11, 25, 29], 22: [2, 5, 8, 28], 23: [11, 20, 26], 24: [10, 13, 15, 29, 30], 25: [4, 14, 19, 21, 29], 26: [1, 7, 10, 11, 18, 23], 27: [0, 6, 14, 15], 28: [1, 6, 8, 11, 12, 13, 15, 17, 22, 30], 29: [4, 5, 9, 10, 12, 17, 21, 24, 25], 30: [1, 6, 7, 10, 12, 13, 17, 24, 28]}</t>
+  </si>
+  <si>
+    <t>{12: 0, 16: 1, 4: 2, 29: 1, 25: 0, 17: 3, 9: 2, 21: 2, 13: 0, 28: 2, 30: 1, 15: 3, 6: 3, 1: 0, 24: 2, 7: 3, 10: 3, 5: 2, 19: 1, 8: 3, 0: 2, 27: 0, 20: 0, 11: 1, 26: 2, 23: 3, 22: 0, 14: 1, 18: 0, 2: 2, 3: 0}</t>
+  </si>
+  <si>
+    <t>{0: [6, 7, 19, 21, 22, 23, 28], 1: [3, 9, 13, 14, 17, 18, 20, 23, 28, 29], 2: [8, 9, 11, 13, 14, 16, 24, 27], 3: [1, 6, 7, 12, 13, 14, 19, 23, 25], 4: [6, 13, 14, 18, 19, 25, 30], 5: [9, 11, 12, 13, 15, 25, 27, 28, 30], 6: [0, 3, 4, 7, 9, 11, 13, 25, 26], 7: [0, 3, 6, 18, 19, 25, 27, 30], 8: [2, 22, 25, 28, 29], 9: [1, 2, 5, 6, 11, 13, 20, 21, 29, 30], 10: [12, 15, 16, 19, 22, 25, 28, 29, 30], 11: [2, 5, 6, 9, 17, 26], 12: [3, 5, 10, 13, 17, 18, 26, 27], 13: [1, 2, 3, 4, 5, 6, 9, 12, 14, 19, 20], 14: [1, 2, 3, 4, 13, 18, 20, 24, 30], 15: [5, 10, 18, 20, 25, 27], 16: [2, 10, 20, 21, 22, 23, 26, 28, 29], 17: [1, 11, 12, 24, 25, 28, 30], 18: [1, 4, 7, 12, 14, 15, 19, 22, 25, 30], 19: [0, 3, 4, 7, 10, 13, 18, 21, 23, 27, 28, 29, 30], 20: [1, 9, 13, 14, 15, 16, 24, 26, 27, 30], 21: [0, 9, 16, 19, 23], 22: [0, 8, 10, 16, 18, 23, 28, 30], 23: [0, 1, 3, 16, 19, 21, 22, 30], 24: [2, 14, 17, 20, 27], 25: [3, 4, 5, 6, 7, 8, 10, 15, 17, 18, 26, 27, 28, 30], 26: [6, 11, 12, 16, 20, 25, 27, 30], 27: [2, 5, 7, 12, 15, 19, 20, 24, 25, 26, 28], 28: [0, 1, 5, 8, 10, 16, 17, 19, 22, 25, 27, 30], 29: [1, 8, 9, 10, 16, 19], 30: [4, 5, 7, 9, 10, 14, 17, 18, 19, 20, 22, 23, 25, 26, 28]}</t>
+  </si>
+  <si>
+    <t>{1: 0, 29: 1, 9: 2, 13: 1, 20: 3, 14: 2, 3: 3, 6: 0, 4: 3, 18: 1, 30: 0, 19: 2, 7: 4, 25: 2, 27: 0, 15: 4, 5: 3, 10: 3, 12: 2, 0: 1, 28: 4, 23: 4, 22: 2, 16: 0, 21: 3, 26: 1, 11: 4, 2: 3, 8: 0, 17: 1, 24: 4}</t>
+  </si>
+  <si>
+    <t>{0: [2, 3, 4, 8, 10, 11, 12, 13, 17, 19, 25, 26, 29], 1: [2, 5, 8, 12, 15, 19, 20, 22, 23, 24, 29, 30], 2: [0, 1, 4, 7, 12, 15, 16, 17, 19, 22], 3: [0, 4, 8, 9, 14, 15, 18, 22, 23, 25, 27], 4: [0, 2, 3, 6, 8, 9, 10, 15, 19, 20, 21, 28, 29], 5: [1, 6, 14, 18, 19, 21, 22, 24, 29], 6: [4, 5, 7, 8, 9, 13, 15, 19, 20, 24, 25], 7: [2, 6, 11, 12, 14, 15, 17, 19, 20, 21, 26, 27, 28, 29], 8: [0, 1, 3, 4, 6, 12, 13, 14, 17, 21, 22, 25, 27], 9: [3, 4, 6, 10, 12, 17, 20, 24, 27, 29, 30], 10: [0, 4, 9, 12, 16, 21, 26], 11: [0, 7, 13, 14, 15, 19, 21, 25, 26], 12: [0, 1, 2, 7, 8, 9, 10, 15, 16, 17, 21, 26, 27], 13: [0, 6, 8, 11, 21, 22, 28, 29, 30], 14: [3, 5, 7, 8, 11, 15, 18, 19, 21, 22, 24, 26, 27], 15: [1, 2, 3, 4, 6, 7, 11, 12, 14, 16, 20, 25, 28], 16: [2, 10, 12, 15, 25, 27, 28, 30], 17: [0, 2, 7, 8, 9, 12, 19, 20, 23, 26, 27, 30], 18: [3, 5, 14, 19, 20, 22, 23, 26, 27, 28, 30], 19: [0, 1, 2, 4, 5, 6, 7, 11, 14, 17, 18, 20, 23, 25, 28, 30], 20: [1, 4, 6, 7, 9, 15, 17, 18, 19, 21, 24, 27], 21: [4, 5, 7, 8, 10, 11, 12, 13, 14, 20, 22, 25], 22: [1, 2, 3, 5, 8, 13, 14, 18, 21, 25, 26, 28, 29, 30], 23: [1, 3, 17, 18, 19], 24: [1, 5, 6, 9, 14, 20, 28, 29], 25: [0, 3, 6, 8, 11, 15, 16, 19, 21, 22, 29], 26: [0, 7, 10, 11, 12, 14, 17, 18, 22, 27], 27: [3, 7, 8, 9, 12, 14, 16, 17, 18, 20, 26], 28: [4, 7, 13, 15, 16, 18, 19, 22, 24, 29], 29: [0, 1, 4, 5, 7, 9, 13, 22, 24, 25, 28], 30: [1, 9, 13, 16, 17, 18, 19, 22]}</t>
+  </si>
+  <si>
+    <t>{8: 0, 25: 1, 22: 2, 21: 3, 3: 3, 14: 1, 13: 1, 0: 2, 5: 0, 18: 4, 19: 3, 30: 0, 27: 2, 28: 0, 7: 4, 6: 2, 15: 5, 12: 1, 17: 5, 2: 0, 1: 4, 9: 4, 11: 0, 26: 3, 4: 1, 20: 0, 10: 0, 24: 3, 29: 5, 16: 3, 23: 0}</t>
+  </si>
+  <si>
+    <t>{0: [1, 3, 4, 5, 6, 8, 9, 14, 15, 17, 19, 23, 25, 26, 27, 28, 29, 30], 1: [0, 2, 4, 8, 9, 14, 15, 16, 17, 18, 19, 22, 23, 24, 26, 28, 30], 2: [1, 4, 7, 8, 12, 13, 14, 15, 16, 17, 20, 23, 28, 30], 3: [0, 4, 5, 6, 8, 10, 11, 15, 17, 18, 19, 20, 21, 22, 23, 24, 26, 27, 29], 4: [0, 1, 2, 3, 7, 10, 15, 16, 18, 21, 24, 25, 26, 27], 5: [0, 3, 6, 9, 12, 14, 16, 18, 19, 21, 22, 23, 24, 25, 26, 28, 30], 6: [0, 3, 5, 8, 11, 13, 14, 17, 18, 20, 21, 22, 25, 26, 27, 28, 30], 7: [2, 4, 8, 9, 11, 15, 16, 17, 19, 20, 22, 23, 24, 26, 27, 28, 30], 8: [0, 1, 2, 3, 6, 7, 15, 16, 20, 22, 27, 29, 30], 9: [0, 1, 5, 7, 10, 11, 13, 16, 19, 20, 23, 26, 27, 28, 30], 10: [3, 4, 9, 12, 13, 14, 17, 20, 22, 23, 25, 26, 27, 28], 11: [3, 6, 7, 9, 12, 18, 19, 21, 22, 25, 26], 12: [2, 5, 10, 11, 14, 16, 18, 19, 24, 25, 26, 27, 28], 13: [2, 6, 9, 10, 14, 20, 21, 22, 28, 30], 14: [0, 1, 2, 5, 6, 10, 12, 13, 15, 18, 19, 21, 23, 24, 28, 30], 15: [0, 1, 2, 3, 4, 7, 8, 14, 18, 23, 30], 16: [1, 2, 4, 5, 7, 8, 9, 12, 19, 21, 23, 25, 27, 28, 30], 17: [0, 1, 2, 3, 6, 7, 10, 20, 22, 23, 24, 25, 27, 29, 30], 18: [1, 3, 4, 5, 6, 11, 12, 14, 15, 19, 26, 27, 28, 30], 19: [0, 1, 3, 5, 7, 9, 11, 12, 14, 16, 18, 20, 21, 22, 26, 29, 30], 20: [2, 3, 6, 7, 8, 9, 10, 13, 17, 19, 25, 26, 30], 21: [3, 4, 5, 6, 11, 13, 14, 16, 19, 22, 24, 25, 26, 28, 29, 30], 22: [1, 3, 5, 6, 7, 8, 10, 11, 13, 17, 19, 21, 24, 26, 27, 28], 23: [0, 1, 2, 3, 5, 7, 9, 10, 14, 15, 16, 17, 24, 25, 26, 27, 28, 29], 24: [1, 3, 4, 5, 7, 12, 14, 17, 21, 22, 23, 27, 29, 30], 25: [0, 4, 5, 6, 10, 11, 12, 16, 17, 20, 21, 23, 26, 28, 29, 30], 26: [0, 1, 3, 4, 5, 6, 7, 9, 10, 11, 12, 18, 19, 20, 21, 22, 23, 25, 28, 29], 27: [0, 3, 4, 6, 7, 8, 9, 10, 12, 16, 17, 18, 22, 23, 24, 28], 28: [0, 1, 2, 5, 6, 7, 9, 10, 12, 13, 14, 16, 18, 21, 22, 23, 25, 26, 27], 29: [0, 3, 8, 17, 19, 21, 23, 24, 25, 26], 30: [0, 1, 2, 5, 6, 7, 8, 9, 13, 14, 15, 16, 17, 18, 19, 20, 21, 24, 25]}</t>
+  </si>
+  <si>
+    <t>{22: 0, 28: 1, 5: 2, 21: 3, 6: 4, 26: 5, 25: 0, 0: 3, 23: 6, 3: 1, 14: 0, 24: 4, 29: 2, 1: 2, 17: 5, 27: 2, 4: 6, 7: 3, 18: 3, 2: 4, 15: 5, 12: 6, 8: 6, 11: 2, 20: 2, 16: 5, 30: 1, 19: 4, 9: 0, 10: 3, 13: 5}</t>
+  </si>
+  <si>
+    <t>{0: [1, 3, 5, 6, 7, 8, 9, 10, 11, 13, 16, 17, 19, 20, 21, 22, 23, 25, 30], 1: [0, 2, 3, 5, 6, 8, 9, 11, 13, 15, 16, 17, 20, 21, 22, 23, 24, 25, 26, 29, 30], 2: [1, 4, 6, 7, 8, 15, 16, 17, 18, 19, 21, 22, 24, 26, 27, 30], 3: [0, 1, 7, 8, 9, 10, 12, 13, 15, 16, 18, 20, 21, 25, 26, 27, 28, 29], 4: [2, 5, 7, 10, 12, 14, 15, 18, 19, 20, 23, 25, 30], 5: [0, 1, 4, 6, 7, 10, 11, 12, 14, 16, 17, 18, 19, 20, 23, 24, 25, 26, 27, 28, 29, 30], 6: [0, 1, 2, 5, 7, 8, 9, 10, 11, 12, 13, 15, 17, 20, 22, 26, 27, 28, 29, 30], 7: [0, 2, 3, 4, 5, 6, 9, 10, 14, 15, 16, 19, 22, 23, 25, 27, 28, 29], 8: [0, 1, 2, 3, 6, 9, 10, 12, 15, 16, 17, 18, 20, 22, 23, 24, 26, 27, 28, 30], 9: [0, 1, 3, 6, 7, 8, 11, 13, 14, 15, 16, 19, 22, 23, 25, 26, 27, 28, 29], 10: [0, 3, 4, 5, 6, 7, 8, 12, 13, 18, 19, 20, 22, 23, 24, 25, 27, 29, 30], 11: [0, 1, 5, 6, 9, 15, 16, 17, 19, 22, 23, 24, 25, 26, 28, 29, 30], 12: [3, 4, 5, 6, 8, 10, 13, 14, 15, 16, 17, 19, 21, 22, 23, 24, 25, 26, 27, 30], 13: [0, 1, 3, 6, 9, 10, 12, 14, 15, 17, 18, 20, 21, 22, 23, 25, 26, 27, 28, 29], 14: [4, 5, 7, 9, 12, 13, 15, 17, 19, 20, 21, 22, 25, 26, 27, 28, 30], 15: [1, 2, 3, 4, 6, 7, 8, 9, 11, 12, 13, 14, 16, 18, 20, 21, 24, 25, 26, 28, 29, 30], 16: [0, 1, 2, 3, 5, 7, 8, 9, 11, 12, 15, 17, 19, 21, 23, 25, 28, 29, 30], 17: [0, 1, 2, 5, 6, 8, 11, 12, 13, 14, 16, 18, 20, 21, 24, 27, 28, 29, 30], 18: [2, 3, 4, 5, 8, 10, 13, 15, 17, 19, 20, 21, 24, 26, 27, 29, 30], 19: [0, 2, 4, 5, 7, 9, 10, 11, 12, 14, 16, 18, 20, 21, 22, 24, 25, 27, 29], 20: [0, 1, 3, 4, 5, 6, 8, 10, 13, 14, 15, 17, 18, 19, 21, 24, 30], 21: [0, 1, 2, 3, 12, 13, 14, 15, 16, 17, 18, 19, 20, 23, 24, 27, 29], 22: [0, 1, 2, 6, 7, 8, 9, 10, 11, 12, 13, 14, 19, 25, 26, 27, 28, 29, 30], 23: [0, 1, 4, 5, 7, 8, 9, 10, 11, 12, 13, 16, 21, 25, 26, 27, 28, 29], 24: [1, 2, 5, 8, 10, 11, 12, 15, 17, 18, 19, 20, 21, 26, 27, 29], 25: [0, 1, 3, 4, 5, 7, 9, 10, 11, 12, 13, 14, 15, 16, 19, 22, 23, 27, 28, 30], 26: [1, 2, 3, 5, 6, 8, 9, 11, 12, 13, 14, 15, 18, 22, 23, 24], 27: [2, 3, 5, 6, 7, 8, 9, 10, 12, 13, 14, 17, 18, 19, 21, 22, 23, 24, 25, 28, 30], 28: [3, 5, 6, 7, 8, 9, 11, 13, 14, 15, 16, 17, 22, 23, 25, 27, 30], 29: [1, 3, 5, 6, 7, 9, 10, 11, 13, 15, 16, 17, 18, 19, 21, 22, 23, 24, 30], 30: [0, 1, 2, 4, 5, 6, 8, 10, 11, 12, 14, 15, 16, 17, 18, 20, 22, 25, 27, 28, 29]}</t>
+  </si>
+  <si>
+    <t>{15: 0, 4: 1, 18: 2, 2: 3, 30: 4, 20: 3, 5: 0, 10: 5, 8: 1, 27: 6, 6: 2, 0: 6, 3: 4, 7: 7, 22: 0, 19: 4, 24: 7, 1: 5, 17: 8, 16: 2, 12: 3, 25: 8, 23: 4, 9: 3, 28: 5, 14: 2, 11: 1, 21: 1, 13: 7, 29: 6, 26: 6}</t>
+  </si>
+  <si>
+    <t>{0: [12, 14, 16], 1: [17, 19, 23], 2: [8, 13, 17, 18], 3: [9, 14, 20, 23, 29], 4: [], 5: [14], 6: [7, 30], 7: [6, 22, 23, 28], 8: [2, 10, 23], 9: [3, 17], 10: [8, 26, 30], 11: [22, 27], 12: [0], 13: [2], 14: [0, 3, 5, 20, 23, 26], 15: [16, 19, 20, 26, 27, 28, 30], 16: [0, 15], 17: [1, 2, 9], 18: [2, 20, 26], 19: [1, 15, 23, 26, 27, 30], 20: [3, 14, 15, 18, 25], 21: [], 22: [7, 11], 23: [1, 3, 7, 8, 14, 19, 26], 24: [26], 25: [20, 30], 26: [10, 14, 15, 18, 19, 23, 24], 27: [11, 15, 19], 28: [7, 15], 29: [3], 30: [6, 10, 15, 19, 25]}</t>
+  </si>
+  <si>
+    <t>{0: 0, 14: 1, 20: 0, 3: 2, 23: 0, 26: 2, 19: 1, 15: 3, 27: 0, 18: 1, 1: 2, 16: 1, 30: 0, 10: 1, 8: 2, 2: 0, 17: 1, 9: 0, 13: 1, 12: 1, 24: 0, 5: 0, 11: 1, 7: 1, 28: 0, 6: 2, 25: 1, 22: 0, 29: 0, 4: 0, 21: 0}</t>
+  </si>
+  <si>
+    <t>{0: [3, 8, 11, 12, 13, 30], 1: [8, 10, 11, 21, 30], 2: [3, 5, 8, 11, 19, 26, 27, 28, 29], 3: [0, 2, 4, 5, 7, 15, 18, 22], 4: [3, 5, 16, 17, 18, 21, 23], 5: [2, 3, 4, 6, 9, 12, 18, 27], 6: [5, 13, 17, 20, 26], 7: [3, 8, 10, 23, 25], 8: [0, 1, 2, 7, 12, 17, 24, 27], 9: [5, 12, 17, 21, 26, 29], 10: [1, 7, 15, 28], 11: [0, 1, 2], 12: [0, 5, 8, 9, 14, 17, 19, 21, 22, 23, 29], 13: [0, 6, 16], 14: [12, 17, 21, 25, 27, 30], 15: [3, 10, 18, 24, 26], 16: [4, 13, 17, 28], 17: [4, 6, 8, 9, 12, 14, 16, 19, 22, 30], 18: [3, 4, 5, 15], 19: [2, 12, 17, 23, 24, 25, 27, 30], 20: [6, 23, 24, 28, 29], 21: [1, 4, 9, 12, 14, 22, 26, 27], 22: [3, 12, 17, 21, 24, 30], 23: [4, 7, 12, 19, 20, 25, 26], 24: [8, 15, 19, 20, 22], 25: [7, 14, 19, 23, 28], 26: [2, 6, 9, 15, 21, 23], 27: [2, 5, 8, 14, 19, 21], 28: [2, 10, 16, 20, 25], 29: [2, 9, 12, 20], 30: [0, 1, 14, 17, 19, 22]}</t>
+  </si>
+  <si>
+    <t>{28: 0, 25: 1, 14: 0, 16: 1, 17: 2, 30: 1, 12: 1, 9: 0, 19: 0, 4: 0, 23: 2, 20: 1, 7: 0, 8: 3, 24: 2, 29: 3, 1: 0, 26: 3, 21: 2, 27: 1, 6: 0, 2: 2, 5: 3, 3: 1, 15: 0, 18: 2, 13: 2, 0: 0, 22: 0, 11: 3, 10: 1}</t>
+  </si>
+  <si>
+    <t>{0: [4, 8, 9, 14, 15, 17, 18, 21, 28], 1: [5, 11, 12, 14, 23, 27, 28, 29, 30], 2: [5, 7, 14, 17, 22, 23, 24, 28, 30], 3: [7, 21, 30], 4: [0, 5, 15, 25], 5: [1, 2, 4, 10, 12, 13, 17, 20, 21, 25, 26, 30], 6: [10, 18, 20, 22, 26, 29, 30], 7: [2, 3, 8, 12, 15, 20, 22, 25], 8: [0, 7, 11, 18, 20, 26, 27], 9: [0, 11, 14, 17, 20, 22, 27, 28, 30], 10: [5, 6, 13, 14, 16, 20, 27, 29], 11: [1, 8, 9, 14, 15, 16, 18, 21, 22, 26, 27], 12: [1, 5, 7, 14, 19, 20, 22, 24], 13: [5, 10, 15, 20, 28], 14: [0, 1, 2, 9, 10, 11, 12, 15, 17, 19, 21], 15: [0, 4, 7, 11, 13, 14, 17, 18, 22, 27, 29], 16: [10, 11, 22, 25, 26, 28], 17: [0, 2, 5, 9, 14, 15, 25, 27, 30], 18: [0, 6, 8, 11, 15, 20, 21, 24, 28], 19: [12, 14, 20, 22], 20: [5, 6, 7, 8, 9, 10, 12, 13, 18, 19, 21, 22, 23, 27], 21: [0, 3, 5, 11, 14, 18, 20, 23, 26, 28, 29], 22: [2, 6, 7, 9, 11, 12, 15, 16, 19, 20], 23: [1, 2, 20, 21, 24, 27, 28], 24: [2, 12, 18, 23, 26, 27, 30], 25: [4, 5, 7, 16, 17, 28, 30], 26: [5, 6, 8, 11, 16, 21, 24, 28], 27: [1, 8, 9, 10, 11, 15, 17, 20, 23, 24, 30], 28: [0, 1, 2, 9, 13, 16, 18, 21, 23, 25, 26], 29: [1, 6, 10, 15, 21, 30], 30: [1, 2, 3, 5, 6, 9, 17, 24, 25, 27, 29]}</t>
+  </si>
+  <si>
+    <t>{4: 0, 0: 1, 15: 2, 14: 0, 17: 3, 9: 2, 25: 1, 5: 2, 2: 1, 30: 0, 27: 1, 1: 3, 11: 4, 21: 3, 18: 0, 28: 4, 20: 4, 12: 1, 10: 3, 22: 0, 7: 3, 16: 2, 8: 2, 23: 0, 13: 0, 19: 2, 6: 1, 29: 4, 26: 0, 3: 1, 24: 2}</t>
+  </si>
+  <si>
+    <t>{0: [1, 2, 3, 5, 15, 16, 17, 19, 21, 26], 1: [0, 4, 5, 13, 16, 19, 20, 21, 24, 26, 28, 29], 2: [0, 3, 4, 7, 9, 15, 17, 21, 22, 25, 26, 27, 30], 3: [0, 2, 9, 11, 15, 16, 17, 18, 21, 22, 25, 28, 30], 4: [1, 2, 5, 6, 8, 10, 13, 16, 18, 20, 30], 5: [0, 1, 4, 7, 8, 10, 11, 18, 22, 24, 25, 26, 28, 29, 30], 6: [4, 9, 11, 15, 18, 20, 23, 25, 28, 30], 7: [2, 5, 12, 15, 16, 19, 22, 23, 26, 28, 29], 8: [4, 5, 9, 15, 16, 19, 20, 21, 22, 23, 24, 26, 30], 9: [2, 3, 6, 8, 15, 17, 23, 24, 27, 28], 10: [4, 5, 11, 12, 13, 15, 17, 19, 21, 26, 28, 29, 30], 11: [3, 5, 6, 10, 14, 19, 23, 25, 28], 12: [7, 10, 16, 17, 23, 25, 26, 27], 13: [1, 4, 10, 17, 26, 29], 14: [11, 16, 18, 19, 21, 22, 23, 25, 27], 15: [0, 2, 3, 6, 7, 8, 9, 10, 20, 21, 22, 27, 29], 16: [0, 1, 3, 4, 7, 8, 12, 14, 18, 21, 24, 27], 17: [0, 2, 3, 9, 10, 12, 13, 18, 20, 21, 23, 25, 26, 27, 28, 29, 30], 18: [3, 4, 5, 6, 14, 16, 17, 24, 26, 27, 28], 19: [0, 1, 7, 8, 10, 11, 14, 24, 26, 27], 20: [1, 4, 6, 8, 15, 17, 22, 23, 25, 29], 21: [0, 1, 2, 3, 8, 10, 14, 15, 16, 17, 22, 24, 26, 27], 22: [2, 3, 5, 7, 8, 14, 15, 20, 21, 23, 24, 25, 28], 23: [6, 7, 8, 9, 11, 12, 14, 17, 20, 22, 26, 27, 30], 24: [1, 5, 8, 9, 16, 18, 19, 21, 22, 27, 28, 29], 25: [2, 3, 5, 6, 11, 12, 14, 17, 20, 22, 27, 28, 29], 26: [0, 1, 2, 5, 7, 8, 10, 12, 13, 17, 18, 19, 21, 23, 27, 28], 27: [2, 9, 12, 14, 15, 16, 17, 18, 19, 21, 23, 24, 25, 26], 28: [1, 3, 5, 6, 7, 9, 10, 11, 17, 18, 22, 24, 25, 26, 30], 29: [1, 5, 7, 10, 13, 15, 17, 20, 24, 25, 30], 30: [2, 3, 4, 5, 6, 8, 10, 17, 23, 28, 29]}</t>
+  </si>
+  <si>
+    <t>{27: 0, 18: 1, 26: 2, 17: 3, 23: 1, 12: 4, 28: 0, 7: 5, 2: 4, 3: 5, 9: 2, 21: 1, 30: 2, 10: 5, 15: 3, 22: 2, 25: 1, 0: 0, 16: 2, 5: 4, 29: 0, 4: 3, 1: 5, 20: 4, 6: 5, 24: 3, 13: 4, 8: 0, 19: 1, 11: 2, 14: 4}</t>
+  </si>
+  <si>
+    <t>{0: [2, 4, 8, 9, 10, 11, 12, 13, 15, 16, 17, 20, 22, 23, 24, 25, 26, 28, 30], 1: [2, 3, 4, 7, 11, 13, 14, 17, 19, 20, 23, 28], 2: [0, 1, 5, 6, 7, 8, 9, 10, 12, 14, 15, 16, 17, 19, 20, 21, 22, 24, 29, 30], 3: [1, 4, 5, 7, 8, 10, 12, 13, 14, 15, 20, 23, 26, 27, 29, 30], 4: [0, 1, 3, 5, 9, 10, 18, 20, 22, 24, 25, 27, 28], 5: [2, 3, 4, 7, 12, 13, 14, 15, 21, 22, 24, 25, 29], 6: [2, 7, 8, 9, 10, 14, 15, 16, 17, 18, 19, 24, 25, 27, 29], 7: [1, 2, 3, 5, 6, 12, 14, 15, 16, 17, 18, 19, 20, 22, 23, 26, 27, 28, 29], 8: [0, 2, 3, 6, 11, 12, 19, 23, 25, 26, 29, 30], 9: [0, 2, 4, 6, 10, 11, 17, 18, 20, 21, 23, 24, 26, 28, 29], 10: [0, 2, 3, 4, 6, 9, 14, 15, 16, 17, 18, 19, 22, 23, 25, 26, 27, 28], 11: [0, 1, 8, 9, 12, 13, 14, 15, 16, 17, 25, 26, 28, 30], 12: [0, 2, 3, 5, 7, 8, 11, 13, 14, 15, 16, 21, 22, 24, 25, 27, 28, 29, 30], 13: [0, 1, 3, 5, 11, 12, 18, 19, 21, 22, 23, 26, 29], 14: [1, 2, 3, 5, 6, 7, 10, 11, 12, 15, 16, 20, 21, 22, 25, 26], 15: [0, 2, 3, 5, 6, 7, 10, 11, 12, 14, 16, 19, 20, 21, 23, 29, 30], 16: [0, 2, 6, 7, 10, 11, 12, 14, 15, 18, 19, 20, 22, 24, 25, 27, 28, 29, 30], 17: [0, 1, 2, 6, 7, 9, 10, 11, 18, 19, 21, 22, 27, 29, 30], 18: [4, 6, 7, 9, 10, 13, 16, 17, 19, 21, 23, 26, 27, 30], 19: [1, 2, 6, 7, 8, 10, 13, 15, 16, 17, 18, 23, 24, 25, 28], 20: [0, 1, 2, 3, 4, 7, 9, 14, 15, 16, 21, 22, 25, 27, 28, 30], 21: [2, 5, 9, 12, 13, 14, 15, 17, 18, 20, 25, 27, 28], 22: [0, 2, 4, 5, 7, 10, 12, 13, 14, 16, 17, 20, 25, 29, 30], 23: [0, 1, 3, 7, 8, 9, 10, 13, 15, 18, 19, 25, 26, 30], 24: [0, 2, 4, 5, 6, 9, 12, 16, 19, 27, 28, 29], 25: [0, 4, 5, 6, 8, 10, 11, 12, 14, 16, 19, 20, 21, 22, 23, 26, 28, 29], 26: [0, 3, 7, 8, 9, 10, 11, 13, 14, 18, 23, 25, 27, 28, 29, 30], 27: [3, 4, 6, 7, 10, 12, 16, 17, 18, 20, 21, 24, 26, 28, 30], 28: [0, 1, 4, 7, 9, 10, 11, 12, 16, 19, 20, 21, 24, 25, 26, 27, 30], 29: [2, 3, 5, 6, 7, 8, 9, 12, 13, 15, 16, 17, 22, 24, 25, 26, 30], 30: [0, 2, 3, 8, 11, 12, 15, 16, 17, 18, 20, 22, 23, 26, 27, 28, 29]}</t>
+  </si>
+  <si>
+    <t>{10: 0, 0: 1, 23: 2, 25: 3, 26: 4, 9: 3, 18: 5, 28: 6, 16: 4, 19: 1, 7: 3, 6: 2, 27: 1, 30: 3, 15: 5, 2: 6, 17: 4, 14: 1, 3: 6, 22: 5, 24: 5, 4: 2, 20: 0, 21: 2, 12: 0, 11: 2, 29: 1, 1: 5, 5: 4, 8: 5, 13: 3}</t>
+  </si>
+  <si>
+    <t>{0: [1, 4, 6, 12, 13, 14, 15, 17, 18, 19, 21, 23, 25, 26, 28, 29, 30], 1: [0, 2, 3, 4, 5, 9, 15, 16, 17, 19, 20, 23, 25, 26, 27, 28, 30], 2: [1, 5, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 20, 23, 25, 26, 27, 28, 30], 3: [1, 4, 5, 6, 8, 10, 12, 13, 14, 15, 16, 17, 20, 21, 22, 23, 25, 26, 27, 30], 4: [0, 1, 3, 5, 7, 8, 9, 10, 11, 12, 15, 17, 18, 19, 20, 23, 24, 26, 27, 28, 29], 5: [1, 2, 3, 4, 8, 10, 11, 13, 14, 15, 20, 21, 22, 24, 25, 26, 27, 29], 6: [0, 3, 7, 8, 9, 11, 12, 13, 15, 16, 17, 18, 19, 21, 23, 26, 27, 28, 29], 7: [4, 6, 8, 9, 10, 16, 20, 21, 22, 23, 24, 25, 27, 28, 30], 8: [3, 4, 5, 6, 7, 9, 11, 12, 13, 16, 17, 18, 19, 20, 21, 23, 25, 28, 30], 9: [1, 2, 4, 6, 7, 8, 11, 14, 19, 20, 22, 23, 25, 26, 27, 29, 30], 10: [2, 3, 4, 5, 7, 13, 14, 15, 16, 17, 18, 19, 20, 21, 23, 25, 26, 29, 30], 11: [2, 4, 5, 6, 8, 9, 12, 13, 14, 15, 17, 18, 19, 20, 21, 25, 26, 27, 30], 12: [0, 2, 3, 4, 6, 8, 11, 14, 16, 18, 22, 24, 25, 26, 27, 28, 29, 30], 13: [0, 2, 3, 5, 6, 8, 10, 11, 14, 18, 20, 21, 22, 25], 14: [0, 2, 3, 5, 9, 10, 11, 12, 13, 15, 18, 20, 22, 24, 27, 29, 30], 15: [0, 1, 2, 3, 4, 5, 6, 10, 11, 14, 16, 18, 19, 23, 24, 25, 26, 30], 16: [1, 2, 3, 6, 7, 8, 10, 12, 15, 18, 20, 21, 22, 23, 27, 28, 29, 30], 17: [0, 1, 2, 3, 4, 6, 8, 10, 11, 18, 19, 22, 23, 24, 26, 28, 29], 18: [0, 2, 4, 6, 8, 10, 11, 12, 13, 14, 15, 16, 17, 19, 20, 21, 22, 24, 26, 27, 28, 29, 30], 19: [0, 1, 4, 6, 8, 9, 10, 11, 15, 17, 18, 21, 23, 25, 27], 20: [1, 2, 3, 4, 5, 7, 8, 9, 10, 11, 13, 14, 16, 18, 21, 23, 27, 29], 21: [0, 3, 5, 6, 7, 8, 10, 11, 13, 16, 18, 19, 20, 23, 24, 25, 27, 29, 30], 22: [3, 5, 7, 9, 12, 13, 14, 16, 17, 18, 23, 25, 26, 28, 29, 30], 23: [0, 1, 2, 3, 4, 6, 7, 8, 9, 10, 15, 16, 17, 19, 20, 21, 22, 26, 28, 29, 30], 24: [4, 5, 7, 12, 14, 15, 17, 18, 21, 25, 27], 25: [0, 1, 2, 3, 5, 7, 8, 9, 10, 11, 12, 13, 15, 19, 21, 22, 24, 28, 29], 26: [0, 1, 2, 3, 4, 5, 6, 9, 10, 11, 12, 15, 17, 18, 22, 23, 27, 28, 29, 30], 27: [1, 2, 3, 4, 5, 6, 7, 9, 11, 12, 14, 16, 18, 19, 20, 21, 24, 26, 28, 30], 28: [0, 1, 2, 4, 6, 7, 8, 12, 16, 17, 18, 22, 23, 25, 26, 27, 29], 29: [0, 4, 5, 6, 9, 10, 12, 14, 16, 17, 18, 20, 21, 22, 23, 25, 26, 28, 30], 30: [0, 1, 2, 3, 7, 8, 9, 10, 11, 12, 14, 15, 16, 18, 21, 22, 23, 26, 27, 29]}</t>
+  </si>
+  <si>
+    <t>{6: 0, 17: 1, 8: 2, 18: 3, 11: 4, 19: 5, 21: 1, 13: 5, 27: 2, 20: 6, 2: 7, 14: 0, 5: 3, 26: 5, 30: 6, 12: 1, 3: 7, 4: 0, 1: 4, 28: 6, 23: 3, 9: 1, 16: 5, 25: 0, 7: 7, 0: 2, 15: 1, 29: 7, 22: 2, 10: 2, 24: 4}</t>
+  </si>
+  <si>
+    <t>{29: 0, 27: 1, 3: 0, 25: 1, 16: 1, 4: 1, 1: 1, 17: 0, 11: 0, 12: 0, 14: 0, 20: 1, 13: 1, 15: 0, 23: 1, 2: 0, 21: 2, 7: 2, 19: 0, 8: 1, 6: 2, 0: 0, 30: 0, 9: 1, 22: 0, 28: 1, 18: 2, 5: 0, 10: 1, 24: 1, 26: 0}</t>
+  </si>
+  <si>
+    <t>{0: [6, 12, 13, 19, 26, 28], 1: [4, 6, 17, 28], 2: [3, 6, 9, 16, 22, 29], 3: [2, 8, 12, 25, 28, 30], 4: [1, 14, 17, 20, 27], 5: [13, 17, 28, 29], 6: [0, 1, 2, 8, 10, 12, 15, 16, 24, 25, 30], 7: [11, 12, 21, 24, 30], 8: [3, 6, 10, 11, 24, 25, 26, 28], 9: [2, 16, 17, 24, 25, 28], 10: [6, 8, 22, 24], 11: [7, 8, 19, 22], 12: [0, 3, 6, 7, 15, 16, 19, 22, 23, 25, 26, 28, 29], 13: [0, 5, 17, 18, 19, 22, 24], 14: [4, 18, 20, 21, 22, 25, 26, 28, 30], 15: [6, 12, 16, 25, 30], 16: [2, 6, 9, 12, 15, 23], 17: [1, 4, 5, 9, 13, 22, 25, 26], 18: [13, 14, 24], 19: [0, 11, 12, 13, 20, 21, 25], 20: [4, 14, 19, 21, 26, 28], 21: [7, 14, 19, 20, 26, 27, 28], 22: [2, 10, 11, 12, 13, 14, 17, 23], 23: [12, 16, 22, 24, 25], 24: [6, 7, 8, 9, 10, 13, 18, 23, 25], 25: [3, 6, 8, 9, 12, 14, 15, 17, 19, 23, 24], 26: [0, 8, 12, 14, 17, 20, 21, 30], 27: [4, 21, 29], 28: [0, 1, 3, 5, 8, 9, 12, 14, 20, 21, 29], 29: [2, 5, 12, 27, 28], 30: [3, 6, 7, 14, 15, 26]}</t>
+  </si>
+  <si>
+    <t>{19: 0, 25: 1, 12: 2, 15: 0, 6: 3, 16: 1, 0: 1, 3: 3, 28: 0, 8: 2, 24: 0, 10: 1, 23: 3, 22: 0, 2: 2, 9: 3, 17: 2, 1: 1, 13: 3, 5: 1, 29: 3, 26: 0, 7: 1, 30: 2, 11: 3, 14: 3, 21: 2, 20: 1, 4: 0, 27: 1, 18: 1}</t>
+  </si>
+  <si>
+    <t>{0: [5, 7, 11, 13, 14, 24, 26], 1: [2, 9, 19, 23, 24, 29], 2: [1, 3, 12, 20, 21, 23, 29], 3: [2, 19, 20, 25, 27], 4: [8, 10, 14, 17, 18, 19, 24, 30], 5: [0, 7, 8, 9, 12, 13, 18, 21, 23, 26, 27, 29, 30], 6: [10, 11, 14, 17, 21, 27, 29], 7: [0, 5, 9, 11, 14, 17, 21, 26, 27, 28], 8: [4, 5, 18, 22, 25, 28, 29, 30], 9: [1, 5, 7, 11, 16, 18, 24, 25, 28, 30], 10: [4, 6, 13, 16, 23, 25, 27, 30], 11: [0, 6, 7, 9, 13, 16, 17, 19, 25, 26, 29], 12: [2, 5, 14, 17, 20, 22, 23, 27], 13: [0, 5, 10, 11, 17, 29], 14: [0, 4, 6, 7, 12, 16, 24, 25, 26, 28, 29], 15: [18, 21, 25, 28], 16: [9, 10, 11, 14, 20, 21, 25, 30], 17: [4, 6, 7, 11, 12, 13, 26], 18: [4, 5, 8, 9, 15, 20, 21, 22, 24, 25], 19: [1, 3, 4, 11, 22, 24, 28, 29], 20: [2, 3, 12, 16, 18, 23, 24, 28, 30], 21: [2, 5, 6, 7, 15, 16, 18, 25, 30], 22: [8, 12, 18, 19, 29], 23: [1, 2, 5, 10, 12, 20], 24: [0, 1, 4, 9, 14, 18, 19, 20, 25, 29, 30], 25: [3, 8, 9, 10, 11, 14, 15, 16, 18, 21, 24], 26: [0, 5, 7, 11, 14, 17, 30], 27: [3, 5, 6, 7, 10, 12, 29, 30], 28: [7, 8, 9, 14, 15, 19, 20], 29: [1, 2, 5, 6, 8, 11, 13, 14, 19, 22, 24, 27, 30], 30: [4, 5, 8, 9, 10, 16, 20, 21, 24, 26, 27, 29]}</t>
+  </si>
+  <si>
+    <t>{22: 0, 18: 1, 8: 2, 5: 0, 21: 2, 25: 0, 15: 3, 16: 1, 30: 3, 9: 2, 24: 4, 29: 1, 4: 0, 27: 2, 10: 4, 19: 2, 13: 2, 6: 0, 20: 0, 1: 0, 28: 1, 14: 3, 0: 1, 7: 4, 11: 3, 17: 1, 12: 4, 2: 3, 26: 2, 23: 1, 3: 1}</t>
+  </si>
+  <si>
+    <t>{0: [2, 8, 10, 11, 18, 20, 25, 30], 1: [2, 4, 7, 8, 9, 11, 15, 18, 23, 24, 27, 28], 2: [0, 1, 6, 8, 13, 14, 17, 18, 19, 23, 29], 3: [5, 8, 9, 12, 13, 14, 18, 20, 21, 26, 30], 4: [1, 5, 9, 14, 17, 19, 20, 28], 5: [3, 4, 6, 7, 9, 10, 12, 13, 15, 16, 17, 22, 23, 27, 30], 6: [2, 5, 7, 8, 12, 14, 21, 22, 26, 28], 7: [1, 5, 6, 9, 10, 11, 12, 13, 14, 15, 16, 20, 23, 27, 28, 30], 8: [0, 1, 2, 3, 6, 10, 12, 15, 18, 20, 21, 22, 23, 25, 26, 27], 9: [1, 3, 4, 5, 7, 10, 15, 16, 20, 21, 22, 24, 28, 30], 10: [0, 5, 7, 8, 9, 11, 12, 13, 15, 17, 18, 20, 21, 23, 27], 11: [0, 1, 7, 10, 13, 14, 17, 18, 19, 22, 23, 24, 25, 26], 12: [3, 5, 6, 7, 8, 10, 15, 20, 21, 23, 24, 25, 26, 27, 28], 13: [2, 3, 5, 7, 10, 11, 14, 16, 17, 21, 27, 29], 14: [2, 3, 4, 6, 7, 11, 13, 17, 18, 19, 21, 22, 24, 25, 28, 29, 30], 15: [1, 5, 7, 8, 9, 10, 12, 18, 19, 24, 29], 16: [5, 7, 9, 13, 24, 26, 30], 17: [2, 4, 5, 10, 11, 13, 14, 18, 19, 21, 22, 24, 28, 29, 30], 18: [0, 1, 2, 3, 8, 10, 11, 14, 15, 17, 20, 22, 30], 19: [2, 4, 11, 14, 15, 17, 20, 26, 30], 20: [0, 3, 4, 7, 8, 9, 10, 12, 18, 19, 24, 29], 21: [3, 6, 8, 9, 10, 12, 13, 14, 17, 22, 27], 22: [5, 6, 8, 9, 11, 14, 17, 18, 21, 23, 26, 27], 23: [1, 2, 5, 7, 8, 10, 11, 12, 22, 26, 27], 24: [1, 9, 11, 12, 14, 15, 16, 17, 20, 25], 25: [0, 8, 11, 12, 14, 24, 26, 27, 29], 26: [3, 6, 8, 11, 12, 16, 19, 22, 23, 25, 30], 27: [1, 5, 7, 8, 10, 12, 13, 21, 22, 23, 25, 30], 28: [1, 4, 6, 7, 9, 12, 14, 17, 29], 29: [2, 13, 14, 15, 17, 20, 25, 28], 30: [0, 3, 5, 7, 9, 14, 16, 17, 18, 19, 26, 27]}</t>
+  </si>
+  <si>
+    <t>{16: 0, 24: 1, 9: 2, 7: 1, 30: 3, 5: 4, 27: 0, 10: 3, 13: 2, 12: 2, 23: 5, 8: 4, 1: 3, 26: 1, 22: 3, 25: 3, 15: 0, 2: 0, 6: 5, 17: 5, 21: 1, 14: 4, 19: 2, 11: 0, 28: 0, 4: 1, 29: 1, 18: 2, 0: 5, 20: 0, 3: 5}</t>
+  </si>
+  <si>
+    <t>{0: [5, 7, 8, 9, 10, 11, 12, 13, 14, 16, 17, 20, 21, 25, 26, 28, 30], 1: [2, 3, 4, 5, 6, 7, 8, 12, 13, 16, 19, 21, 22, 23, 24, 26, 27, 29, 30], 2: [1, 3, 4, 8, 10, 14, 16, 17, 18, 20, 21, 23, 26, 28, 29, 30], 3: [1, 2, 10, 14, 16, 17, 18, 19, 22, 23, 25, 27, 28, 29, 30], 4: [1, 2, 5, 9, 10, 12, 13, 16, 18, 19, 20, 21, 26, 29, 30], 5: [0, 1, 4, 6, 8, 13, 15, 17, 18, 19, 20, 22, 24, 25, 27, 28], 6: [1, 5, 8, 9, 10, 12, 13, 14, 15, 17, 20, 23, 24, 25, 27, 30], 7: [0, 1, 8, 11, 12, 14, 18, 20, 21, 22, 23, 24, 28, 29, 30], 8: [0, 1, 2, 5, 6, 7, 9, 13, 17, 18, 19, 21, 23, 25, 26, 30], 9: [0, 4, 6, 8, 11, 15, 16, 17, 18, 20, 23, 24, 25, 28], 10: [0, 2, 3, 4, 6, 12, 14, 15, 16, 17, 26, 30], 11: [0, 7, 9, 12, 15, 16, 17, 18, 20, 21, 22, 24, 26, 30], 12: [0, 1, 4, 6, 7, 10, 11, 13, 14, 15, 17, 20, 22, 25, 26, 28, 29], 13: [0, 1, 4, 5, 6, 8, 12, 15, 18, 19, 25, 26, 27, 28], 14: [0, 2, 3, 6, 7, 10, 12, 17, 19, 22, 25, 26, 28, 30], 15: [5, 6, 9, 10, 11, 12, 13, 17, 19, 20, 28], 16: [0, 1, 2, 3, 4, 9, 10, 11, 19, 20, 21, 22, 23, 24, 25, 26, 27, 29], 17: [0, 2, 3, 5, 6, 8, 9, 10, 11, 12, 14, 15, 19, 20, 21, 23, 24, 25, 26, 27, 28], 18: [2, 3, 4, 5, 7, 8, 9, 11, 13, 20, 21, 22, 23, 24, 25, 29, 30], 19: [1, 3, 4, 5, 8, 13, 14, 15, 16, 17, 20, 22, 23, 24, 26, 28], 20: [0, 2, 4, 5, 6, 7, 9, 11, 12, 15, 16, 17, 18, 19, 24, 26, 29, 30], 21: [0, 1, 2, 4, 7, 8, 11, 16, 17, 18, 22, 24, 27, 29, 30], 22: [1, 3, 5, 7, 11, 12, 14, 16, 18, 19, 21, 23, 24], 23: [1, 2, 3, 6, 7, 8, 9, 16, 17, 18, 19, 22, 24, 26], 24: [1, 5, 6, 7, 9, 11, 16, 17, 18, 19, 20, 21, 22, 23, 27, 28, 29], 25: [0, 3, 5, 6, 8, 9, 12, 13, 14, 16, 17, 18, 26, 27], 26: [0, 1, 2, 4, 8, 10, 11, 12, 13, 14, 16, 17, 19, 20, 23, 25, 28, 29, 30], 27: [1, 3, 5, 6, 13, 16, 17, 21, 24, 25, 29], 28: [0, 2, 3, 5, 7, 9, 12, 13, 14, 15, 17, 19, 24, 26], 29: [1, 2, 3, 4, 7, 12, 16, 18, 20, 21, 24, 26, 27], 30: [0, 1, 2, 3, 4, 6, 7, 8, 10, 11, 14, 18, 20, 21, 26]}</t>
+  </si>
+  <si>
+    <t>{0: 0, 12: 1, 13: 2, 26: 3, 28: 4, 14: 2, 17: 5, 10: 4, 25: 4, 8: 1, 30: 5, 4: 0, 19: 6, 1: 4, 5: 3, 2: 6, 18: 7, 15: 0, 20: 2, 29: 5, 11: 4, 23: 0, 24: 1, 22: 5, 16: 7, 9: 3, 27: 0, 6: 6, 3: 1, 21: 2, 7: 3}</t>
+  </si>
+  <si>
+    <t>{0: [1, 2, 4, 5, 6, 7, 9, 11, 12, 13, 14, 15, 18, 21, 23, 24, 25, 27, 28], 1: [0, 2, 3, 5, 6, 7, 9, 11, 12, 13, 14, 15, 18, 20, 21, 22, 24, 25, 28, 29, 30], 2: [0, 1, 3, 6, 8, 9, 10, 13, 14, 15, 16, 17, 18, 23, 28, 29, 30], 3: [1, 2, 4, 6, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 23, 24, 25, 26, 27, 28, 30], 4: [0, 3, 5, 6, 9, 11, 12, 16, 18, 19, 20, 25, 27, 28, 29, 30], 5: [0, 1, 4, 8, 12, 13, 15, 17, 18, 20, 21, 22, 23, 26, 28, 29, 30], 6: [0, 1, 2, 3, 4, 7, 8, 9, 10, 11, 12, 13, 16, 19, 20, 25, 27, 28, 29], 7: [0, 1, 6, 8, 9, 10, 11, 13, 14, 16, 18, 19, 20, 21, 22, 23, 28, 29, 30], 8: [2, 5, 6, 7, 10, 11, 12, 14, 15, 16, 18, 19, 21, 22, 25, 27, 28, 29, 30], 9: [0, 1, 2, 3, 4, 6, 7, 10, 12, 13, 14, 15, 16, 17, 21, 22, 23, 24, 26, 29, 30], 10: [2, 3, 6, 7, 8, 9, 14, 16, 17, 18, 20, 22, 23, 25, 26, 27, 30], 11: [0, 1, 3, 4, 6, 7, 8, 12, 13, 18, 19, 20, 23, 26, 28, 30], 12: [0, 1, 3, 4, 5, 6, 8, 9, 11, 13, 14, 15, 16, 18, 19, 21, 24, 25, 26, 27, 30], 13: [0, 1, 2, 3, 5, 6, 7, 9, 11, 12, 15, 17, 18, 19, 22, 23, 24, 26, 27, 29], 14: [0, 1, 2, 3, 7, 8, 9, 10, 12, 15, 16, 19, 20, 22, 26, 27, 28], 15: [0, 1, 2, 3, 5, 8, 9, 12, 13, 14, 17, 18, 19, 21, 26, 27, 29], 16: [2, 3, 4, 6, 7, 8, 9, 10, 12, 14, 18, 19, 20, 22, 24, 25, 27, 28, 29], 17: [2, 3, 5, 9, 10, 13, 15, 23, 24, 26, 28, 29, 30], 18: [0, 1, 2, 3, 4, 5, 7, 8, 10, 11, 12, 13, 15, 16, 19, 20, 21, 23, 26, 27, 29], 19: [3, 4, 6, 7, 8, 11, 12, 13, 14, 15, 16, 18, 20, 21, 23, 25, 26, 27, 28, 29, 30], 20: [1, 4, 5, 6, 7, 10, 11, 14, 16, 18, 19, 21, 22, 23, 25, 30], 21: [0, 1, 5, 7, 8, 9, 12, 15, 18, 19, 20, 22, 23, 24, 26, 28, 29, 30], 22: [1, 5, 7, 8, 9, 10, 13, 14, 16, 20, 21, 23, 25, 28, 29, 30], 23: [0, 2, 3, 5, 7, 9, 10, 11, 13, 17, 18, 19, 20, 21, 22, 25, 26, 27, 28, 29, 30], 24: [0, 1, 3, 9, 12, 13, 16, 17, 21, 28, 30], 25: [0, 1, 3, 4, 6, 8, 10, 12, 16, 19, 20, 22, 23, 26, 28, 29], 26: [3, 5, 9, 10, 11, 12, 13, 14, 15, 17, 18, 19, 21, 23, 25, 27], 27: [0, 3, 4, 6, 8, 10, 12, 13, 14, 15, 16, 18, 19, 23, 26, 29, 30], 28: [0, 1, 2, 3, 4, 5, 6, 7, 8, 11, 14, 16, 17, 19, 21, 22, 23, 24, 25, 30], 29: [1, 2, 4, 5, 6, 7, 8, 9, 13, 15, 16, 17, 18, 19, 21, 22, 23, 25, 27], 30: [1, 2, 3, 4, 5, 7, 8, 9, 10, 11, 12, 17, 19, 20, 21, 22, 23, 24, 27, 28]}</t>
+  </si>
+  <si>
+    <t>{1: 0, 6: 1, 25: 2, 28: 3, 3: 4, 11: 2, 12: 3, 13: 5, 18: 1, 0: 4, 7: 6, 19: 0, 23: 7, 26: 6, 27: 2, 5: 2, 21: 5, 30: 1, 9: 2, 15: 7, 2: 6, 22: 4, 8: 8, 29: 3, 16: 5, 14: 1, 20: 3, 10: 0, 17: 8, 24: 6, 4: 6}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +341,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -150,12 +374,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -201,11 +425,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,9 +512,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -244,6 +528,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -255,6 +542,70 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,7 +732,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Results!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -404,24 +755,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:f>Results!$B$15:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>148</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>152</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,7 +789,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>Results!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -461,24 +812,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$F$16</c:f>
+              <c:f>Results!$B$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>108</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -913,7 +1264,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$23</c:f>
+              <c:f>Results!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,24 +1287,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$F$23</c:f>
+              <c:f>Results!$B$23:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>1042</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19893</c:v>
+                  <c:v>1129</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>154</c:v>
+                  <c:v>898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>274</c:v>
+                  <c:v>1710</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>589</c:v>
+                  <c:v>1361</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -970,7 +1321,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$24</c:f>
+              <c:f>Results!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -993,24 +1344,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$F$24</c:f>
+              <c:f>Results!$B$24:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>81</c:v>
+                  <c:v>846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16925</c:v>
+                  <c:v>902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93</c:v>
+                  <c:v>743</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>193</c:v>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>467</c:v>
+                  <c:v>1157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1445,7 +1796,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$31</c:f>
+              <c:f>Results!$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1468,24 +1819,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$31:$F$31</c:f>
+              <c:f>Results!$B$31:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2551</c:v>
+                  <c:v>253457</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16933</c:v>
+                  <c:v>5681</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5389</c:v>
+                  <c:v>12285</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14950</c:v>
+                  <c:v>5424</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4407</c:v>
+                  <c:v>1038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1502,7 +1853,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$32</c:f>
+              <c:f>Results!$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1525,24 +1876,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$32:$F$32</c:f>
+              <c:f>Results!$B$32:$F$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2026</c:v>
+                  <c:v>211700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14678</c:v>
+                  <c:v>4634</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4434</c:v>
+                  <c:v>10510</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12028</c:v>
+                  <c:v>5330</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3654</c:v>
+                  <c:v>764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1972,7 +2323,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$39</c:f>
+              <c:f>Results!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1995,24 +2346,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$39:$F$39</c:f>
+              <c:f>Results!$B$39:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>80567</c:v>
+                  <c:v>36881</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39302</c:v>
+                  <c:v>18587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54602</c:v>
+                  <c:v>14479</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12545</c:v>
+                  <c:v>51857</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69103</c:v>
+                  <c:v>6986520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2029,7 +2380,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$40</c:f>
+              <c:f>Results!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2052,24 +2403,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$40:$F$40</c:f>
+              <c:f>Results!$B$40:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>67853</c:v>
+                  <c:v>30201</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33346</c:v>
+                  <c:v>15164</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43640</c:v>
+                  <c:v>12440</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10644</c:v>
+                  <c:v>42114</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57126</c:v>
+                  <c:v>5926680</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2504,7 +2855,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$47</c:f>
+              <c:f>Results!$A$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2527,24 +2878,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$47:$F$47</c:f>
+              <c:f>Results!$B$47:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>456827</c:v>
+                  <c:v>3842630</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5594237</c:v>
+                  <c:v>73949</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1380314</c:v>
+                  <c:v>24224240</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29281831</c:v>
+                  <c:v>490451</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2980276</c:v>
+                  <c:v>15665371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2561,7 +2912,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$48</c:f>
+              <c:f>Results!$A$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2584,24 +2935,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$48:$F$48</c:f>
+              <c:f>Results!$B$48:$F$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>376609</c:v>
+                  <c:v>3270313</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4666384</c:v>
+                  <c:v>55951</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1099275</c:v>
+                  <c:v>19529759</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24789700</c:v>
+                  <c:v>406326</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2406045</c:v>
+                  <c:v>13218189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5777,13 +6128,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>332154</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>181708</xdr:rowOff>
+      <xdr:rowOff>194408</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>361461</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>52754</xdr:rowOff>
+      <xdr:rowOff>65454</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6180,10 +6531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFCA1D8-37C5-FA4D-BDD1-DACA3CAE6D4E}">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6193,10 +6544,13 @@
     <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="3.1640625" style="19" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="8" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
@@ -6211,8 +6565,9 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M1" s="19"/>
+    </row>
+    <row r="2" spans="1:25" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>17</v>
       </c>
@@ -6228,7 +6583,7 @@
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
     </row>
-    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
@@ -6243,8 +6598,18 @@
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
-    </row>
-    <row r="4" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+    </row>
+    <row r="4" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -6277,21 +6642,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
@@ -6305,175 +6670,199 @@
       </c>
       <c r="J5" s="1">
         <f>MAX(B5:F5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="1">
         <f>AVERAGE(B5:F5)</f>
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="L5" s="1">
         <f>MEDIAN(B5:F5)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="10">
-        <v>3.15213203430175E-3</v>
-      </c>
-      <c r="C6" s="10">
-        <v>3.3636093139648398E-3</v>
-      </c>
-      <c r="D6" s="10">
-        <v>3.0789375305175699E-3</v>
-      </c>
-      <c r="E6" s="10">
-        <v>3.9579868316650304E-3</v>
-      </c>
-      <c r="F6" s="10">
-        <v>2.8841495513915998E-3</v>
+      <c r="B6" s="9">
+        <v>6.2620639801025304E-3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4.4400691986083898E-3</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5.0990581512451102E-3</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2.64787673950195E-2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>7.0538520812988203E-3</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ref="I6:I9" si="0">MIN(B6:F6)</f>
-        <v>2.8841495513915998E-3</v>
+        <v>4.4400691986083898E-3</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" ref="J6:J9" si="1">MAX(B6:F6)</f>
-        <v>3.9579868316650304E-3</v>
+        <v>2.64787673950195E-2</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" ref="K6:K9" si="2">AVERAGE(B6:F6)</f>
-        <v>3.2873630523681577E-3</v>
+        <v>9.86676216125487E-3</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ref="L6:L9" si="3">MEDIAN(B6:F6)</f>
-        <v>3.15213203430175E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6.2620639801025304E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1">
-        <v>40</v>
+        <v>229</v>
       </c>
       <c r="F7" s="1">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>229</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>43.6</v>
+        <v>84.2</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="F8" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>170</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>12.6</v>
+        <v>47.2</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>43.2</v>
+        <v>44</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+    </row>
+    <row r="11" spans="1:25" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>11</v>
       </c>
@@ -6489,7 +6878,7 @@
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
     </row>
-    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -6522,7 +6911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
@@ -6561,164 +6950,178 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="10">
-        <v>9.7098350524902292E-3</v>
-      </c>
-      <c r="C14" s="10">
-        <v>4.6918392181396398E-3</v>
-      </c>
-      <c r="D14" s="10">
-        <v>7.3800086975097604E-3</v>
-      </c>
-      <c r="E14" s="10">
-        <v>1.7014980316162099E-2</v>
-      </c>
-      <c r="F14" s="10">
-        <v>5.38396835327148E-3</v>
+      <c r="B14" s="9">
+        <v>1.2144088745117101E-2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>9.6020698547363195E-3</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1.6933917999267498E-2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>4.4301033020019497E-2</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1.37348175048828E-2</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" ref="I14:I17" si="4">MIN(B14:F14)</f>
-        <v>4.6918392181396398E-3</v>
+        <v>9.6020698547363195E-3</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" ref="J14:J17" si="5">MAX(B14:F14)</f>
-        <v>1.7014980316162099E-2</v>
+        <v>4.4301033020019497E-2</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" ref="K14:K17" si="6">AVERAGE(B14:F14)</f>
-        <v>8.8361263275146418E-3</v>
+        <v>1.9343185424804642E-2</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" ref="L14:L17" si="7">MEDIAN(B14:F14)</f>
-        <v>7.3800086975097604E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1.37348175048828E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="E15" s="1">
-        <v>149</v>
+        <v>200</v>
       </c>
       <c r="F15" s="1">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="4"/>
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="5"/>
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="K15" s="1">
         <f t="shared" si="6"/>
-        <v>120.4</v>
+        <v>113.6</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="7"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="E16" s="1">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="F16" s="1">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="4"/>
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="5"/>
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" si="6"/>
-        <v>79.400000000000006</v>
+        <v>68.2</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="7"/>
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D17" s="1">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E17" s="1">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F17" s="1">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="4"/>
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" si="6"/>
-        <v>92.2</v>
+        <v>94.6</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="7"/>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>12</v>
       </c>
@@ -6734,7 +7137,7 @@
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
     </row>
-    <row r="20" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -6767,15 +7170,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1">
         <v>5</v>
@@ -6791,11 +7194,11 @@
       </c>
       <c r="I21" s="1">
         <f>MIN(B21:F21)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J21" s="1">
         <f>MAX(B21:F21)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K21" s="1">
         <f>AVERAGE(B21:F21)</f>
@@ -6806,164 +7209,178 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="10">
-        <v>6.3190460205078099E-3</v>
-      </c>
-      <c r="C22" s="11">
-        <v>0.92105865478515603</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1.29919052124023E-2</v>
-      </c>
-      <c r="E22" s="10">
-        <v>2.6300191879272398E-2</v>
-      </c>
-      <c r="F22" s="10">
-        <v>5.0382852554321199E-2</v>
+      <c r="B22" s="9">
+        <v>7.9633235931396401E-2</v>
+      </c>
+      <c r="C22" s="10">
+        <v>9.1376066207885701E-2</v>
+      </c>
+      <c r="D22" s="9">
+        <v>9.0371131896972601E-2</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.21761894226074199</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.15629696846008301</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" ref="I22:I25" si="8">MIN(B22:F22)</f>
-        <v>6.3190460205078099E-3</v>
+        <v>7.9633235931396401E-2</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" ref="J22:J25" si="9">MAX(B22:F22)</f>
-        <v>0.92105865478515603</v>
+        <v>0.21761894226074199</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" ref="K22:K25" si="10">AVERAGE(B22:F22)</f>
-        <v>0.20341053009033194</v>
+        <v>0.12705926895141595</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" ref="L22:L25" si="11">MEDIAN(B22:F22)</f>
-        <v>2.6300191879272398E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9.1376066207885701E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="1">
-        <v>128</v>
+        <v>1042</v>
       </c>
       <c r="C23" s="1">
-        <v>19893</v>
+        <v>1129</v>
       </c>
       <c r="D23" s="1">
-        <v>154</v>
+        <v>898</v>
       </c>
       <c r="E23" s="1">
-        <v>274</v>
+        <v>1710</v>
       </c>
       <c r="F23" s="1">
-        <v>589</v>
+        <v>1361</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="8"/>
-        <v>128</v>
+        <v>898</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="9"/>
-        <v>19893</v>
+        <v>1710</v>
       </c>
       <c r="K23" s="1">
         <f t="shared" si="10"/>
-        <v>4207.6000000000004</v>
+        <v>1228</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="11"/>
-        <v>274</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="1">
-        <v>81</v>
+        <v>846</v>
       </c>
       <c r="C24" s="1">
-        <v>16925</v>
+        <v>902</v>
       </c>
       <c r="D24" s="1">
-        <v>93</v>
+        <v>743</v>
       </c>
       <c r="E24" s="1">
-        <v>193</v>
+        <v>1440</v>
       </c>
       <c r="F24" s="1">
-        <v>467</v>
+        <v>1157</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="8"/>
-        <v>81</v>
+        <v>743</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="9"/>
-        <v>16925</v>
+        <v>1440</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="10"/>
-        <v>3551.8</v>
+        <v>1017.6</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="11"/>
-        <v>193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C25" s="1">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D25" s="1">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E25" s="1">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F25" s="1">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="8"/>
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="9"/>
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="10"/>
-        <v>134.6</v>
+        <v>133.4</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="11"/>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+    </row>
+    <row r="27" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>13</v>
       </c>
@@ -6979,7 +7396,7 @@
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
     </row>
-    <row r="28" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>1</v>
       </c>
@@ -7012,12 +7429,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1">
         <v>6</v>
@@ -7040,152 +7457,152 @@
       </c>
       <c r="J29" s="1">
         <f>MAX(B29:F29)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K29" s="1">
         <f>AVERAGE(B29:F29)</f>
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="L29" s="1">
         <f>MEDIAN(B29:F29)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="10">
-        <v>0.131369829177856</v>
-      </c>
-      <c r="C30" s="10">
-        <v>1.0380160808563199</v>
-      </c>
-      <c r="D30" s="10">
-        <v>0.35393095016479398</v>
-      </c>
-      <c r="E30" s="10">
-        <v>0.83887100219726496</v>
-      </c>
-      <c r="F30" s="10">
-        <v>0.30499982833862299</v>
+      <c r="B30" s="9">
+        <v>12.729412078857401</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.33175778388977001</v>
+      </c>
+      <c r="D30" s="9">
+        <v>1.1133108139037999</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0.85305690765380804</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0.23129224777221599</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" ref="I30:I33" si="12">MIN(B30:F30)</f>
-        <v>0.131369829177856</v>
+        <v>0.23129224777221599</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" ref="J30:J33" si="13">MAX(B30:F30)</f>
-        <v>1.0380160808563199</v>
+        <v>12.729412078857401</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" ref="K30:K33" si="14">AVERAGE(B30:F30)</f>
-        <v>0.53343753814697159</v>
+        <v>3.0517659664153993</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" ref="L30:L33" si="15">MEDIAN(B30:F30)</f>
-        <v>0.35393095016479398</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0.85305690765380804</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="1">
-        <v>2551</v>
-      </c>
-      <c r="C31" s="10">
-        <v>16933</v>
+        <v>253457</v>
+      </c>
+      <c r="C31" s="9">
+        <v>5681</v>
       </c>
       <c r="D31" s="1">
-        <v>5389</v>
+        <v>12285</v>
       </c>
       <c r="E31" s="1">
-        <v>14950</v>
+        <v>5424</v>
       </c>
       <c r="F31" s="1">
-        <v>4407</v>
+        <v>1038</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="12"/>
-        <v>2551</v>
+        <v>1038</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="13"/>
-        <v>16933</v>
+        <v>253457</v>
       </c>
       <c r="K31" s="1">
         <f t="shared" si="14"/>
-        <v>8846</v>
+        <v>55577</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="15"/>
-        <v>5389</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>5681</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="1">
-        <v>2026</v>
+        <v>211700</v>
       </c>
       <c r="C32" s="1">
-        <v>14678</v>
+        <v>4634</v>
       </c>
       <c r="D32" s="1">
-        <v>4434</v>
+        <v>10510</v>
       </c>
       <c r="E32" s="1">
-        <v>12028</v>
+        <v>5330</v>
       </c>
       <c r="F32" s="1">
-        <v>3654</v>
+        <v>764</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="12"/>
-        <v>2026</v>
+        <v>764</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="13"/>
-        <v>14678</v>
+        <v>211700</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="14"/>
-        <v>7364</v>
+        <v>46587.6</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="15"/>
-        <v>4434</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>5330</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="1">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="C33" s="1">
+        <v>187</v>
+      </c>
+      <c r="D33" s="1">
         <v>170</v>
       </c>
-      <c r="D33" s="1">
-        <v>173</v>
-      </c>
       <c r="E33" s="1">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F33" s="1">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>10</v>
@@ -7196,19 +7613,33 @@
       </c>
       <c r="J33" s="1">
         <f t="shared" si="13"/>
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" si="14"/>
-        <v>182.2</v>
+        <v>186.4</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="15"/>
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+    </row>
+    <row r="35" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>14</v>
       </c>
@@ -7224,7 +7655,7 @@
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
     </row>
-    <row r="36" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>1</v>
       </c>
@@ -7257,11 +7688,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="9">
         <v>7</v>
       </c>
       <c r="C37" s="1">
@@ -7274,7 +7705,7 @@
         <v>7</v>
       </c>
       <c r="F37" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>9</v>
@@ -7285,152 +7716,152 @@
       </c>
       <c r="J37" s="1">
         <f>MAX(B37:F37)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K37" s="1">
         <f>AVERAGE(B37:F37)</f>
-        <v>7</v>
+        <v>7.2</v>
       </c>
       <c r="L37" s="1">
         <f>MEDIAN(B37:F37)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="10">
-        <v>4.6643912792205802</v>
-      </c>
-      <c r="C38" s="10">
-        <v>2.0657799243927002</v>
-      </c>
-      <c r="D38" s="11">
-        <v>4.9732720851898096</v>
-      </c>
-      <c r="E38" s="10">
-        <v>0.85173106193542403</v>
-      </c>
-      <c r="F38" s="10">
-        <v>7.9749341011047301</v>
+      <c r="B38" s="9">
+        <v>2.4901762008666899</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1.0043480396270701</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1.14838695526123</v>
+      </c>
+      <c r="E38" s="9">
+        <v>7.37235260009765</v>
+      </c>
+      <c r="F38" s="9">
+        <v>456.560941934585</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" ref="I38:I41" si="16">MIN(B38:F38)</f>
-        <v>0.85173106193542403</v>
+        <v>1.0043480396270701</v>
       </c>
       <c r="J38" s="1">
         <f t="shared" ref="J38:J41" si="17">MAX(B38:F38)</f>
-        <v>7.9749341011047301</v>
+        <v>456.560941934585</v>
       </c>
       <c r="K38" s="1">
         <f t="shared" ref="K38:K41" si="18">AVERAGE(B38:F38)</f>
-        <v>4.1060216903686486</v>
+        <v>93.715241146087536</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" ref="L38:L41" si="19">MEDIAN(B38:F38)</f>
-        <v>4.6643912792205802</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2.4901762008666899</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B39" s="1">
-        <v>80567</v>
-      </c>
-      <c r="C39" s="10">
-        <v>39302</v>
+        <v>36881</v>
+      </c>
+      <c r="C39" s="9">
+        <v>18587</v>
       </c>
       <c r="D39" s="1">
-        <v>54602</v>
+        <v>14479</v>
       </c>
       <c r="E39" s="1">
-        <v>12545</v>
-      </c>
-      <c r="F39" s="1">
-        <v>69103</v>
+        <v>51857</v>
+      </c>
+      <c r="F39" s="9">
+        <v>6986520</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" si="16"/>
-        <v>12545</v>
+        <v>14479</v>
       </c>
       <c r="J39" s="1">
         <f t="shared" si="17"/>
-        <v>80567</v>
+        <v>6986520</v>
       </c>
       <c r="K39" s="1">
         <f t="shared" si="18"/>
-        <v>51223.8</v>
+        <v>1421664.8</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="19"/>
-        <v>54602</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+        <v>36881</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B40" s="1">
-        <v>67853</v>
-      </c>
-      <c r="C40" s="10">
-        <v>33346</v>
+        <v>30201</v>
+      </c>
+      <c r="C40" s="9">
+        <v>15164</v>
       </c>
       <c r="D40" s="1">
-        <v>43640</v>
+        <v>12440</v>
       </c>
       <c r="E40" s="1">
-        <v>10644</v>
-      </c>
-      <c r="F40" s="1">
-        <v>57126</v>
+        <v>42114</v>
+      </c>
+      <c r="F40" s="9">
+        <v>5926680</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" si="16"/>
-        <v>10644</v>
+        <v>12440</v>
       </c>
       <c r="J40" s="1">
         <f t="shared" si="17"/>
-        <v>67853</v>
+        <v>5926680</v>
       </c>
       <c r="K40" s="1">
         <f t="shared" si="18"/>
-        <v>42521.8</v>
+        <v>1205319.8</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" si="19"/>
-        <v>43640</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+        <v>30201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B41" s="1">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C41" s="1">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D41" s="1">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="E41" s="1">
-        <v>231</v>
-      </c>
-      <c r="F41" s="8">
-        <v>229</v>
+        <v>242</v>
+      </c>
+      <c r="F41" s="7">
+        <v>238</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>10</v>
@@ -7441,19 +7872,33 @@
       </c>
       <c r="J41" s="1">
         <f t="shared" si="17"/>
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="K41" s="1">
         <f t="shared" si="18"/>
-        <v>230.8</v>
+        <v>236.8</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="19"/>
-        <v>230</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+    </row>
+    <row r="43" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>15</v>
       </c>
@@ -7469,7 +7914,7 @@
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
     </row>
-    <row r="44" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>1</v>
       </c>
@@ -7502,21 +7947,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B45" s="1">
+        <v>9</v>
+      </c>
+      <c r="C45" s="1">
         <v>8</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="9">
         <v>9</v>
       </c>
-      <c r="D45" s="1">
-        <v>9</v>
-      </c>
       <c r="E45" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" s="1">
         <v>9</v>
@@ -7534,128 +7979,128 @@
       </c>
       <c r="K45" s="1">
         <f>AVERAGE(B45:F45)</f>
-        <v>8.8000000000000007</v>
+        <v>8.6</v>
       </c>
       <c r="L45" s="1">
         <f>MEDIAN(B45:F45)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="10">
-        <v>25.7871830463409</v>
-      </c>
-      <c r="C46" s="10">
-        <v>377.88461303710898</v>
-      </c>
-      <c r="D46" s="10">
-        <v>109.210680007934</v>
-      </c>
-      <c r="E46" s="10">
-        <v>1760.6418681144701</v>
-      </c>
-      <c r="F46" s="10">
-        <v>277.79642701148902</v>
+      <c r="B46" s="9">
+        <v>340.59954214096001</v>
+      </c>
+      <c r="C46" s="9">
+        <v>8.6951758861541695</v>
+      </c>
+      <c r="D46" s="9">
+        <v>1529.2090008258799</v>
+      </c>
+      <c r="E46" s="9">
+        <v>63.311522006988497</v>
+      </c>
+      <c r="F46" s="9">
+        <v>991.40959382057099</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" ref="I46:I49" si="20">MIN(B46:F46)</f>
-        <v>25.7871830463409</v>
+        <v>8.6951758861541695</v>
       </c>
       <c r="J46" s="1">
         <f t="shared" ref="J46:J49" si="21">MAX(B46:F46)</f>
-        <v>1760.6418681144701</v>
+        <v>1529.2090008258799</v>
       </c>
       <c r="K46" s="1">
         <f t="shared" ref="K46:K49" si="22">AVERAGE(B46:F46)</f>
-        <v>510.26415424346862</v>
+        <v>586.64496693611068</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" ref="L46:L49" si="23">MEDIAN(B46:F46)</f>
-        <v>277.79642701148902</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+        <v>340.59954214096001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B47" s="1">
-        <v>456827</v>
-      </c>
-      <c r="C47" s="10">
-        <v>5594237</v>
-      </c>
-      <c r="D47" s="10">
-        <v>1380314</v>
-      </c>
-      <c r="E47" s="10">
-        <v>29281831</v>
+        <v>3842630</v>
+      </c>
+      <c r="C47" s="9">
+        <v>73949</v>
+      </c>
+      <c r="D47" s="9">
+        <v>24224240</v>
+      </c>
+      <c r="E47" s="9">
+        <v>490451</v>
       </c>
       <c r="F47" s="1">
-        <v>2980276</v>
+        <v>15665371</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="20"/>
-        <v>456827</v>
+        <v>73949</v>
       </c>
       <c r="J47" s="1">
         <f t="shared" si="21"/>
-        <v>29281831</v>
+        <v>24224240</v>
       </c>
       <c r="K47" s="1">
         <f t="shared" si="22"/>
-        <v>7938697</v>
+        <v>8859328.1999999993</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="23"/>
-        <v>2980276</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3842630</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B48" s="1">
-        <v>376609</v>
-      </c>
-      <c r="C48" s="10">
-        <v>4666384</v>
-      </c>
-      <c r="D48" s="10">
-        <v>1099275</v>
-      </c>
-      <c r="E48" s="10">
-        <v>24789700</v>
+        <v>3270313</v>
+      </c>
+      <c r="C48" s="9">
+        <v>55951</v>
+      </c>
+      <c r="D48" s="9">
+        <v>19529759</v>
+      </c>
+      <c r="E48" s="9">
+        <v>406326</v>
       </c>
       <c r="F48" s="1">
-        <v>2406045</v>
+        <v>13218189</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" si="20"/>
-        <v>376609</v>
+        <v>55951</v>
       </c>
       <c r="J48" s="1">
         <f t="shared" si="21"/>
-        <v>24789700</v>
+        <v>19529759</v>
       </c>
       <c r="K48" s="1">
         <f t="shared" si="22"/>
-        <v>6667602.5999999996</v>
+        <v>7296107.5999999996</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" si="23"/>
-        <v>2406045</v>
+        <v>3270313</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -7663,158 +8108,164 @@
         <v>10</v>
       </c>
       <c r="B49" s="1">
-        <v>275</v>
-      </c>
-      <c r="C49" s="10">
+        <v>274</v>
+      </c>
+      <c r="C49" s="9">
         <v>291</v>
       </c>
-      <c r="D49" s="10">
-        <v>297</v>
+      <c r="D49" s="9">
+        <v>288</v>
       </c>
       <c r="E49" s="1">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F49" s="1">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" si="20"/>
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J49" s="1">
         <f t="shared" si="21"/>
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="K49" s="1">
         <f t="shared" si="22"/>
-        <v>287.8</v>
+        <v>282.8</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" si="23"/>
-        <v>291</v>
-      </c>
-    </row>
-    <row r="65" spans="10:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="J65" s="14" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="K65" s="22"/>
+      <c r="L65" s="22"/>
+      <c r="M65" s="23"/>
+    </row>
+    <row r="66" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="24"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="24"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="24"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="24"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="24"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="21"/>
+      <c r="M71" s="24"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J72" s="21"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="21"/>
+      <c r="M72" s="24"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="24"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="24"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="24"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J76" s="21"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="21"/>
+      <c r="M76" s="24"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J77" s="21"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="21"/>
+      <c r="M77" s="24"/>
+    </row>
+    <row r="78" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-    </row>
-    <row r="66" spans="10:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J66" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-    </row>
-    <row r="67" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-    </row>
-    <row r="68" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-    </row>
-    <row r="69" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
-      <c r="M69" s="13"/>
-    </row>
-    <row r="70" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-    </row>
-    <row r="71" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-    </row>
-    <row r="72" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="13"/>
-    </row>
-    <row r="73" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-    </row>
-    <row r="74" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-    </row>
-    <row r="75" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-    </row>
-    <row r="76" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-    </row>
-    <row r="77" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-    </row>
-    <row r="78" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-    </row>
-    <row r="79" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="13"/>
-    </row>
-    <row r="80" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="24"/>
+    </row>
+    <row r="79" spans="1:13" ht="253" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
+      <c r="M79" s="24"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J80" s="21"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="24"/>
     </row>
     <row r="81" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="12"/>
-      <c r="K81" s="12"/>
-      <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
+      <c r="K81" s="11"/>
+      <c r="L81" s="11"/>
+      <c r="M81" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="J66:M80"/>
-    <mergeCell ref="J65:M65"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:L3"/>
@@ -7823,8 +8274,507 @@
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A35:L35"/>
     <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="A79:E79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E550EA22-51CB-4440-97FB-98E18AA4A82D}">
+  <dimension ref="A1:L48"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="35"/>
+    <col min="2" max="2" width="164" style="35" customWidth="1"/>
+    <col min="3" max="3" width="76.6640625" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="32">
+        <v>2</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="32">
+        <v>3</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="32">
+        <v>4</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="32">
+        <v>5</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:12" s="41" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+    </row>
+    <row r="11" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="32">
+        <v>1</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="32">
+        <v>2</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="32">
+        <v>3</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" s="32">
+        <v>4</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="32">
+        <v>5</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="38"/>
+    </row>
+    <row r="18" spans="1:3" s="41" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+    </row>
+    <row r="19" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" s="32">
+        <v>1</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A21" s="32">
+        <v>2</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A22" s="32">
+        <v>3</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="32">
+        <v>4</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A24" s="32">
+        <v>5</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
+    </row>
+    <row r="26" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A26" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+    </row>
+    <row r="27" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A28" s="32">
+        <v>1</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A29" s="32">
+        <v>2</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A30" s="32">
+        <v>3</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A31" s="32">
+        <v>4</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A32" s="32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:3" ht="24" x14ac:dyDescent="0.2">
+      <c r="A34" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+    </row>
+    <row r="35" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A36" s="32">
+        <v>1</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A37" s="32">
+        <v>2</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A38" s="32">
+        <v>3</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A39" s="32">
+        <v>4</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A40" s="32">
+        <v>5</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:3" s="41" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A42" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+    </row>
+    <row r="43" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A44" s="32">
+        <v>1</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A45" s="32">
+        <v>2</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A46" s="32">
+        <v>3</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A47" s="32">
+        <v>4</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A48" s="32">
+        <v>5</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>